<commit_message>
Removed star variants from attributes
Will use the star variant as the value for a gene instead of the star
variant as an attribute, since the same star variant is associated with
multiple genes.
</commit_message>
<xml_diff>
--- a/MHGR/Data/EAVAttributes/EAVAttributes.xlsx
+++ b/MHGR/Data/EAVAttributes/EAVAttributes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke Rasmussen\Dropbox\MMI\Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\MHGR\MHGR\Data\EAVAttributes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="87">
   <si>
     <t>Name</t>
   </si>
@@ -161,39 +161,6 @@
     <t>Clopidogrel metabolism</t>
   </si>
   <si>
-    <t>*1</t>
-  </si>
-  <si>
-    <t>*2</t>
-  </si>
-  <si>
-    <t>*3</t>
-  </si>
-  <si>
-    <t>*4</t>
-  </si>
-  <si>
-    <t>*5</t>
-  </si>
-  <si>
-    <t>*6</t>
-  </si>
-  <si>
-    <t>*7</t>
-  </si>
-  <si>
-    <t>*8</t>
-  </si>
-  <si>
-    <t>*9</t>
-  </si>
-  <si>
-    <t>*10</t>
-  </si>
-  <si>
-    <t>*17</t>
-  </si>
-  <si>
     <t>rs12248560</t>
   </si>
   <si>
@@ -312,6 +279,9 @@
   </si>
   <si>
     <t>rs397515963</t>
+  </si>
+  <si>
+    <t>Gene result type</t>
   </si>
 </sst>
 </file>
@@ -654,17 +624,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75:B78"/>
+    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="48.90625" customWidth="1"/>
     <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.81640625" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -678,10 +649,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -710,7 +681,7 @@
         <v>2</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G65" si="0">CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A3, ", '", B3, "', '", C3, "', ", IF(D3 = "", "NULL", CONCATENATE("'", D3, "'")), ", ", IF(E3 = "", "NULL", CONCATENATE("'", E3, "'")), ")")</f>
+        <f t="shared" ref="G3:G54" si="0">CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A3, ", '", B3, "', '", C3, "', ", IF(D3 = "", "NULL", CONCATENATE("'", D3, "'")), ", ", IF(E3 = "", "NULL", CONCATENATE("'", E3, "'")), ")")</f>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (2, 'Is a', 'binary', NULL, NULL)</v>
       </c>
     </row>
@@ -953,7 +924,7 @@
         <v>289.81</v>
       </c>
       <c r="E19" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
@@ -974,7 +945,7 @@
         <v>289.81</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
@@ -1010,7 +981,7 @@
         <v>289.81</v>
       </c>
       <c r="E22" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
@@ -1031,7 +1002,7 @@
         <v>289.81</v>
       </c>
       <c r="E23" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
@@ -1067,7 +1038,7 @@
         <v>289.81</v>
       </c>
       <c r="E25" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
@@ -1088,7 +1059,7 @@
         <v>425.1</v>
       </c>
       <c r="E26" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
@@ -1109,7 +1080,7 @@
         <v>425.1</v>
       </c>
       <c r="E27" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
@@ -1130,7 +1101,7 @@
         <v>425.1</v>
       </c>
       <c r="E28" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
@@ -1151,7 +1122,7 @@
         <v>425.1</v>
       </c>
       <c r="E29" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
@@ -1202,7 +1173,7 @@
         <v>2621</v>
       </c>
       <c r="E32" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="0"/>
@@ -1223,7 +1194,7 @@
         <v>2623</v>
       </c>
       <c r="E33" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="0"/>
@@ -1244,7 +1215,7 @@
         <v>23663</v>
       </c>
       <c r="E34" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="0"/>
@@ -1265,7 +1236,7 @@
         <v>3535</v>
       </c>
       <c r="E35" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="0"/>
@@ -1286,7 +1257,7 @@
         <v>3542</v>
       </c>
       <c r="E36" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="0"/>
@@ -1307,7 +1278,7 @@
         <v>7577</v>
       </c>
       <c r="E37" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="0"/>
@@ -1328,7 +1299,7 @@
         <v>7551</v>
       </c>
       <c r="E38" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="0"/>
@@ -1349,7 +1320,7 @@
         <v>11949</v>
       </c>
       <c r="E39" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="0"/>
@@ -1370,7 +1341,7 @@
         <v>12010</v>
       </c>
       <c r="E40" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
@@ -1385,11 +1356,17 @@
         <v>46</v>
       </c>
       <c r="C41" t="s">
-        <v>2</v>
+        <v>61</v>
+      </c>
+      <c r="D41" t="s">
+        <v>46</v>
+      </c>
+      <c r="E41" t="s">
+        <v>66</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (40, '*1', 'binary', NULL, NULL)</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (40, 'rs12248560', 'short_text', 'rs12248560', 'dbSNP')</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
@@ -1400,11 +1377,17 @@
         <v>47</v>
       </c>
       <c r="C42" t="s">
-        <v>2</v>
+        <v>61</v>
+      </c>
+      <c r="D42" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" t="s">
+        <v>66</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (41, '*2', 'binary', NULL, NULL)</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (41, 'rs28399504', 'short_text', 'rs28399504', 'dbSNP')</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
@@ -1415,11 +1398,17 @@
         <v>48</v>
       </c>
       <c r="C43" t="s">
-        <v>2</v>
+        <v>61</v>
+      </c>
+      <c r="D43" t="s">
+        <v>48</v>
+      </c>
+      <c r="E43" t="s">
+        <v>66</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (42, '*3', 'binary', NULL, NULL)</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (42, 'rs41291556', 'short_text', 'rs41291556', 'dbSNP')</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
@@ -1430,11 +1419,17 @@
         <v>49</v>
       </c>
       <c r="C44" t="s">
-        <v>2</v>
+        <v>61</v>
+      </c>
+      <c r="D44" t="s">
+        <v>49</v>
+      </c>
+      <c r="E44" t="s">
+        <v>66</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (43, '*4', 'binary', NULL, NULL)</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (43, 'rs72558184', 'short_text', 'rs72558184', 'dbSNP')</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
@@ -1445,11 +1440,17 @@
         <v>50</v>
       </c>
       <c r="C45" t="s">
-        <v>2</v>
+        <v>61</v>
+      </c>
+      <c r="D45" t="s">
+        <v>50</v>
+      </c>
+      <c r="E45" t="s">
+        <v>66</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (44, '*5', 'binary', NULL, NULL)</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (44, 'rs4986893', 'short_text', 'rs4986893', 'dbSNP')</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
@@ -1460,11 +1461,17 @@
         <v>51</v>
       </c>
       <c r="C46" t="s">
-        <v>2</v>
+        <v>61</v>
+      </c>
+      <c r="D46" t="s">
+        <v>51</v>
+      </c>
+      <c r="E46" t="s">
+        <v>66</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (45, '*6', 'binary', NULL, NULL)</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (45, 'rs4244285', 'short_text', 'rs4244285', 'dbSNP')</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
@@ -1475,11 +1482,17 @@
         <v>52</v>
       </c>
       <c r="C47" t="s">
-        <v>2</v>
+        <v>61</v>
+      </c>
+      <c r="D47" t="s">
+        <v>52</v>
+      </c>
+      <c r="E47" t="s">
+        <v>66</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (46, '*7', 'binary', NULL, NULL)</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (46, 'rs72558186', 'short_text', 'rs72558186', 'dbSNP')</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
@@ -1490,11 +1503,17 @@
         <v>53</v>
       </c>
       <c r="C48" t="s">
-        <v>2</v>
+        <v>61</v>
+      </c>
+      <c r="D48" t="s">
+        <v>53</v>
+      </c>
+      <c r="E48" t="s">
+        <v>66</v>
       </c>
       <c r="G48" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (47, '*8', 'binary', NULL, NULL)</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (47, 'rs56337013', 'short_text', 'rs56337013', 'dbSNP')</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
@@ -1505,11 +1524,17 @@
         <v>54</v>
       </c>
       <c r="C49" t="s">
-        <v>2</v>
+        <v>61</v>
+      </c>
+      <c r="D49" t="s">
+        <v>54</v>
+      </c>
+      <c r="E49" t="s">
+        <v>66</v>
       </c>
       <c r="G49" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (48, '*9', 'binary', NULL, NULL)</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (48, 'rs17884712', 'short_text', 'rs17884712', 'dbSNP')</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
@@ -1520,11 +1545,17 @@
         <v>55</v>
       </c>
       <c r="C50" t="s">
-        <v>2</v>
+        <v>61</v>
+      </c>
+      <c r="D50" t="s">
+        <v>55</v>
+      </c>
+      <c r="E50" t="s">
+        <v>66</v>
       </c>
       <c r="G50" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (49, '*10', 'binary', NULL, NULL)</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (49, 'rs6413438', 'short_text', 'rs6413438', 'dbSNP')</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
@@ -1535,11 +1566,17 @@
         <v>56</v>
       </c>
       <c r="C51" t="s">
-        <v>2</v>
+        <v>61</v>
+      </c>
+      <c r="D51" t="s">
+        <v>56</v>
+      </c>
+      <c r="E51" t="s">
+        <v>66</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (50, '*17', 'binary', NULL, NULL)</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (50, 'rs1057910', 'short_text', 'rs1057910', 'dbSNP')</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
@@ -1550,17 +1587,17 @@
         <v>57</v>
       </c>
       <c r="C52" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D52" t="s">
         <v>57</v>
       </c>
       <c r="E52" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (51, 'rs12248560', 'short_text', 'rs12248560', 'dbSNP')</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (51, 'rs1799853', 'short_text', 'rs1799853', 'dbSNP')</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
@@ -1571,17 +1608,17 @@
         <v>58</v>
       </c>
       <c r="C53" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D53" t="s">
         <v>58</v>
       </c>
       <c r="E53" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G53" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (52, 'rs28399504', 'short_text', 'rs28399504', 'dbSNP')</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (52, 'rs9923231', 'short_text', 'rs9923231', 'dbSNP')</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
@@ -1592,17 +1629,17 @@
         <v>59</v>
       </c>
       <c r="C54" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D54" t="s">
         <v>59</v>
       </c>
       <c r="E54" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G54" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (53, 'rs41291556', 'short_text', 'rs41291556', 'dbSNP')</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (53, 'rs9934438', 'short_text', 'rs9934438', 'dbSNP')</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
@@ -1613,17 +1650,17 @@
         <v>60</v>
       </c>
       <c r="C55" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D55" t="s">
         <v>60</v>
       </c>
       <c r="E55" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G55" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (54, 'rs72558184', 'short_text', 'rs72558184', 'dbSNP')</v>
+        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A55, ", '", B55, "', '", C72, "', ", IF(D55 = "", "NULL", CONCATENATE("'", D55, "'")), ", ", IF(E55 = "", "NULL", CONCATENATE("'", E55, "'")), ")")</f>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (54, 'rs8050894', 'short_text', 'rs8050894', 'dbSNP')</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
@@ -1631,20 +1668,20 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
+        <v>69</v>
+      </c>
+      <c r="C56" t="s">
         <v>61</v>
       </c>
-      <c r="C56" t="s">
-        <v>72</v>
-      </c>
       <c r="D56" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="E56" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G56" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (55, 'rs4986893', 'short_text', 'rs4986893', 'dbSNP')</v>
+        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A56, ", '", B56, "', '", C73, "', ", IF(D56 = "", "NULL", CONCATENATE("'", D56, "'")), ", ", IF(E56 = "", "NULL", CONCATENATE("'", E56, "'")), ")")</f>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (55, 'rs6025', 'date_time', 'rs6025', 'dbSNP')</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
@@ -1652,20 +1689,20 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C57" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D57" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="E57" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G57" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (56, 'rs4244285', 'short_text', 'rs4244285', 'dbSNP')</v>
+        <f t="shared" ref="G57:G74" si="1">CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A57, ", '", B57, "', '", C74, "', ", IF(D57 = "", "NULL", CONCATENATE("'", D57, "'")), ", ", IF(E57 = "", "NULL", CONCATENATE("'", E57, "'")), ")")</f>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (56, 'rs1799963', 'short_text', 'rs1799963', 'dbSNP')</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
@@ -1673,20 +1710,20 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C58" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D58" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E58" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G58" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (57, 'rs72558186', 'short_text', 'rs72558186', 'dbSNP')</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (57, 'rs121913626', '', 'rs121913626', 'dbSNP')</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
@@ -1694,20 +1731,20 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C59" t="s">
+        <v>61</v>
+      </c>
+      <c r="D59" t="s">
         <v>72</v>
       </c>
-      <c r="D59" t="s">
-        <v>64</v>
-      </c>
       <c r="E59" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G59" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (58, 'rs56337013', 'short_text', 'rs56337013', 'dbSNP')</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (58, 'rs3218713', '', 'rs3218713', 'dbSNP')</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
@@ -1715,20 +1752,20 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C60" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D60" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="E60" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G60" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (59, 'rs17884712', 'short_text', 'rs17884712', 'dbSNP')</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (59, 'rs3218714', '', 'rs3218714', 'dbSNP')</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
@@ -1736,20 +1773,20 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
+        <v>74</v>
+      </c>
+      <c r="C61" t="s">
+        <v>61</v>
+      </c>
+      <c r="D61" t="s">
+        <v>74</v>
+      </c>
+      <c r="E61" t="s">
         <v>66</v>
       </c>
-      <c r="C61" t="s">
-        <v>72</v>
-      </c>
-      <c r="D61" t="s">
-        <v>66</v>
-      </c>
-      <c r="E61" t="s">
-        <v>77</v>
-      </c>
       <c r="G61" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (60, 'rs6413438', 'short_text', 'rs6413438', 'dbSNP')</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (60, 'rs121964855', '', 'rs121964855', 'dbSNP')</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
@@ -1757,20 +1794,20 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C62" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D62" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="E62" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G62" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (61, 'rs1057910', 'short_text', 'rs1057910', 'dbSNP')</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (61, 'rs121964856', '', 'rs121964856', 'dbSNP')</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
@@ -1778,20 +1815,20 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C63" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D63" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="E63" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G63" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (62, 'rs1799853', 'short_text', 'rs1799853', 'dbSNP')</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (62, 'rs121964857', '', 'rs121964857', 'dbSNP')</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
@@ -1799,20 +1836,20 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="C64" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D64" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="E64" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G64" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (63, 'rs9923231', 'short_text', 'rs9923231', 'dbSNP')</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (63, 'rs28934269', '', 'rs28934269', 'dbSNP')</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
@@ -1820,20 +1857,20 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C65" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D65" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="E65" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G65" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (64, 'rs9934438', 'short_text', 'rs9934438', 'dbSNP')</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (64, 'rs28934270', '', 'rs28934270', 'dbSNP')</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
@@ -1841,20 +1878,20 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C66" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D66" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="E66" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G66" t="str">
-        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A66, ", '", B66, "', '", C83, "', ", IF(D66 = "", "NULL", CONCATENATE("'", D66, "'")), ", ", IF(E66 = "", "NULL", CONCATENATE("'", E66, "'")), ")")</f>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (65, 'rs8050894', 'short_text', 'rs8050894', 'dbSNP')</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (65, 'rs727504290', '', 'rs727504290', 'dbSNP')</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
@@ -1865,17 +1902,17 @@
         <v>80</v>
       </c>
       <c r="C67" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D67" t="s">
         <v>80</v>
       </c>
       <c r="E67" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G67" t="str">
-        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A67, ", '", B67, "', '", C84, "', ", IF(D67 = "", "NULL", CONCATENATE("'", D67, "'")), ", ", IF(E67 = "", "NULL", CONCATENATE("'", E67, "'")), ")")</f>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (66, 'rs6025', 'date_time', 'rs6025', 'dbSNP')</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (66, 'rs104894504', '', 'rs104894504', 'dbSNP')</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
@@ -1886,17 +1923,17 @@
         <v>81</v>
       </c>
       <c r="C68" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D68" t="s">
         <v>81</v>
       </c>
       <c r="E68" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G68" t="str">
-        <f t="shared" ref="G68:G84" si="1">CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A68, ", '", B68, "', '", C85, "', ", IF(D68 = "", "NULL", CONCATENATE("'", D68, "'")), ", ", IF(E68 = "", "NULL", CONCATENATE("'", E68, "'")), ")")</f>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (67, 'rs1799963', '', 'rs1799963', 'dbSNP')</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (67, 'rs375882485', '', 'rs375882485', 'dbSNP')</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
@@ -1907,17 +1944,17 @@
         <v>82</v>
       </c>
       <c r="C69" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D69" t="s">
         <v>82</v>
       </c>
       <c r="E69" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G69" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (68, 'rs121913626', '', 'rs121913626', 'dbSNP')</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (68, 'rs397516083', '', 'rs397516083', 'dbSNP')</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
@@ -1928,17 +1965,17 @@
         <v>83</v>
       </c>
       <c r="C70" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D70" t="s">
         <v>83</v>
       </c>
       <c r="E70" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G70" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (69, 'rs3218713', '', 'rs3218713', 'dbSNP')</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (69, 'rs397515937', '', 'rs397515937', 'dbSNP')</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
@@ -1949,17 +1986,17 @@
         <v>84</v>
       </c>
       <c r="C71" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D71" t="s">
         <v>84</v>
       </c>
       <c r="E71" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G71" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (70, 'rs3218714', '', 'rs3218714', 'dbSNP')</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (70, 'rs397516074', '', 'rs397516074', 'dbSNP')</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
@@ -1970,17 +2007,17 @@
         <v>85</v>
       </c>
       <c r="C72" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D72" t="s">
         <v>85</v>
       </c>
       <c r="E72" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G72" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (71, 'rs121964855', '', 'rs121964855', 'dbSNP')</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (71, 'rs397515963', '', 'rs397515963', 'dbSNP')</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
@@ -1988,20 +2025,14 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="C73" t="s">
-        <v>72</v>
-      </c>
-      <c r="D73" t="s">
-        <v>86</v>
-      </c>
-      <c r="E73" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="G73" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (72, 'rs121964856', '', 'rs121964856', 'dbSNP')</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (72, 'Resulted on', '', NULL, NULL)</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
@@ -2009,224 +2040,14 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C74" t="s">
-        <v>72</v>
-      </c>
-      <c r="D74" t="s">
-        <v>87</v>
-      </c>
-      <c r="E74" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="G74" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (73, 'rs121964857', '', 'rs121964857', 'dbSNP')</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A75">
-        <v>74</v>
-      </c>
-      <c r="B75" t="s">
-        <v>88</v>
-      </c>
-      <c r="C75" t="s">
-        <v>72</v>
-      </c>
-      <c r="D75" t="s">
-        <v>88</v>
-      </c>
-      <c r="E75" t="s">
-        <v>77</v>
-      </c>
-      <c r="G75" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (74, 'rs28934269', '', 'rs28934269', 'dbSNP')</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A76">
-        <v>75</v>
-      </c>
-      <c r="B76" t="s">
-        <v>89</v>
-      </c>
-      <c r="C76" t="s">
-        <v>72</v>
-      </c>
-      <c r="D76" t="s">
-        <v>89</v>
-      </c>
-      <c r="E76" t="s">
-        <v>77</v>
-      </c>
-      <c r="G76" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (75, 'rs28934270', '', 'rs28934270', 'dbSNP')</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A77">
-        <v>76</v>
-      </c>
-      <c r="B77" t="s">
-        <v>90</v>
-      </c>
-      <c r="C77" t="s">
-        <v>72</v>
-      </c>
-      <c r="D77" t="s">
-        <v>90</v>
-      </c>
-      <c r="E77" t="s">
-        <v>77</v>
-      </c>
-      <c r="G77" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (76, 'rs727504290', '', 'rs727504290', 'dbSNP')</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A78">
-        <v>77</v>
-      </c>
-      <c r="B78" t="s">
-        <v>91</v>
-      </c>
-      <c r="C78" t="s">
-        <v>72</v>
-      </c>
-      <c r="D78" t="s">
-        <v>91</v>
-      </c>
-      <c r="E78" t="s">
-        <v>77</v>
-      </c>
-      <c r="G78" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (77, 'rs104894504', '', 'rs104894504', 'dbSNP')</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A79">
-        <v>78</v>
-      </c>
-      <c r="B79" t="s">
-        <v>92</v>
-      </c>
-      <c r="C79" t="s">
-        <v>72</v>
-      </c>
-      <c r="D79" t="s">
-        <v>92</v>
-      </c>
-      <c r="E79" t="s">
-        <v>77</v>
-      </c>
-      <c r="G79" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (78, 'rs375882485', '', 'rs375882485', 'dbSNP')</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A80">
-        <v>79</v>
-      </c>
-      <c r="B80" t="s">
-        <v>93</v>
-      </c>
-      <c r="C80" t="s">
-        <v>72</v>
-      </c>
-      <c r="D80" t="s">
-        <v>93</v>
-      </c>
-      <c r="E80" t="s">
-        <v>77</v>
-      </c>
-      <c r="G80" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (79, 'rs397516083', '', 'rs397516083', 'dbSNP')</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A81">
-        <v>80</v>
-      </c>
-      <c r="B81" t="s">
-        <v>94</v>
-      </c>
-      <c r="C81" t="s">
-        <v>72</v>
-      </c>
-      <c r="D81" t="s">
-        <v>94</v>
-      </c>
-      <c r="E81" t="s">
-        <v>77</v>
-      </c>
-      <c r="G81" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (80, 'rs397515937', '', 'rs397515937', 'dbSNP')</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A82">
-        <v>81</v>
-      </c>
-      <c r="B82" t="s">
-        <v>95</v>
-      </c>
-      <c r="C82" t="s">
-        <v>72</v>
-      </c>
-      <c r="D82" t="s">
-        <v>95</v>
-      </c>
-      <c r="E82" t="s">
-        <v>77</v>
-      </c>
-      <c r="G82" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (81, 'rs397516074', '', 'rs397516074', 'dbSNP')</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A83">
-        <v>82</v>
-      </c>
-      <c r="B83" t="s">
-        <v>96</v>
-      </c>
-      <c r="C83" t="s">
-        <v>72</v>
-      </c>
-      <c r="D83" t="s">
-        <v>96</v>
-      </c>
-      <c r="E83" t="s">
-        <v>77</v>
-      </c>
-      <c r="G83" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (82, 'rs397515963', '', 'rs397515963', 'dbSNP')</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A84">
-        <v>83</v>
-      </c>
-      <c r="B84" t="s">
-        <v>78</v>
-      </c>
-      <c r="C84" t="s">
-        <v>79</v>
-      </c>
-      <c r="G84" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (83, 'Resulted on', '', NULL, NULL)</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (73, 'Gene result type', '', NULL, NULL)</v>
       </c>
     </row>
   </sheetData>
@@ -2239,8 +2060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E121" sqref="E121"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A123" sqref="A123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2286,7 +2107,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E66" si="0">CONCATENATE("INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (", A3, ", ", B3, ", ", C3, ")")</f>
+        <f t="shared" ref="E3:E57" si="0">CONCATENATE("INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (", A3, ", ", B3, ", ", C3, ")")</f>
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (3, 1, 2)</v>
       </c>
     </row>
@@ -3111,7 +2932,7 @@
         <v>5</v>
       </c>
       <c r="E58" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E58:E121" si="1">CONCATENATE("INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (", A58, ", ", B58, ", ", C58, ")")</f>
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (40, 31, 5)</v>
       </c>
     </row>
@@ -3126,7 +2947,7 @@
         <v>5</v>
       </c>
       <c r="E59" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (41, 31, 5)</v>
       </c>
     </row>
@@ -3141,7 +2962,7 @@
         <v>5</v>
       </c>
       <c r="E60" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (42, 31, 5)</v>
       </c>
     </row>
@@ -3156,7 +2977,7 @@
         <v>5</v>
       </c>
       <c r="E61" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (43, 31, 5)</v>
       </c>
     </row>
@@ -3171,7 +2992,7 @@
         <v>5</v>
       </c>
       <c r="E62" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (44, 31, 5)</v>
       </c>
     </row>
@@ -3186,7 +3007,7 @@
         <v>5</v>
       </c>
       <c r="E63" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (45, 31, 5)</v>
       </c>
     </row>
@@ -3201,7 +3022,7 @@
         <v>5</v>
       </c>
       <c r="E64" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (46, 31, 5)</v>
       </c>
     </row>
@@ -3216,7 +3037,7 @@
         <v>5</v>
       </c>
       <c r="E65" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (47, 31, 5)</v>
       </c>
     </row>
@@ -3231,7 +3052,7 @@
         <v>5</v>
       </c>
       <c r="E66" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (48, 31, 5)</v>
       </c>
     </row>
@@ -3246,7 +3067,7 @@
         <v>5</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" ref="E67:E121" si="1">CONCATENATE("INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (", A67, ", ", B67, ", ", C67, ")")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (49, 31, 5)</v>
       </c>
     </row>
@@ -3255,19 +3076,19 @@
         <v>50</v>
       </c>
       <c r="B68">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C68">
         <v>5</v>
       </c>
       <c r="E68" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (50, 31, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (50, 32, 5)</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B69">
         <v>32</v>
@@ -3277,42 +3098,42 @@
       </c>
       <c r="E69" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (40, 32, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (51, 32, 5)</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B70">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C70">
         <v>5</v>
       </c>
       <c r="E70" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (41, 32, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (52, 33, 5)</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B71">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C71">
         <v>5</v>
       </c>
       <c r="E71" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (42, 32, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (53, 33, 5)</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="B72">
         <v>33</v>
@@ -3322,749 +3143,749 @@
       </c>
       <c r="E72" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (40, 33, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (54, 33, 5)</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="B73">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C73">
         <v>5</v>
       </c>
       <c r="E73" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (41, 33, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (55, 35, 5)</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="B74">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C74">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E74" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 40, 6)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (56, 34, 5)</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="B75">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C75">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E75" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 41, 6)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (57, 36, 5)</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="B76">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C76">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E76" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 42, 6)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (58, 36, 5)</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="B77">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C77">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E77" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 43, 6)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (59, 36, 5)</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A78">
-        <v>31</v>
-      </c>
-      <c r="B78">
-        <v>44</v>
-      </c>
-      <c r="C78">
-        <v>6</v>
-      </c>
-      <c r="E78" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 44, 6)</v>
+      <c r="A78" s="1">
+        <v>60</v>
+      </c>
+      <c r="B78" s="1">
+        <v>38</v>
+      </c>
+      <c r="C78" s="1">
+        <v>5</v>
+      </c>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (60, 38, 5)</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A79">
-        <v>31</v>
-      </c>
-      <c r="B79">
-        <v>45</v>
-      </c>
-      <c r="C79">
-        <v>6</v>
-      </c>
-      <c r="E79" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 45, 6)</v>
+      <c r="A79" s="1">
+        <v>61</v>
+      </c>
+      <c r="B79" s="1">
+        <v>38</v>
+      </c>
+      <c r="C79" s="1">
+        <v>5</v>
+      </c>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (61, 38, 5)</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A80">
-        <v>31</v>
-      </c>
-      <c r="B80">
-        <v>46</v>
-      </c>
-      <c r="C80">
-        <v>6</v>
-      </c>
-      <c r="E80" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 46, 6)</v>
+      <c r="A80" s="1">
+        <v>62</v>
+      </c>
+      <c r="B80" s="1">
+        <v>38</v>
+      </c>
+      <c r="C80" s="1">
+        <v>5</v>
+      </c>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (62, 38, 5)</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A81">
-        <v>31</v>
-      </c>
-      <c r="B81">
-        <v>47</v>
-      </c>
-      <c r="C81">
-        <v>6</v>
-      </c>
-      <c r="E81" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 47, 6)</v>
+      <c r="A81" s="1">
+        <v>63</v>
+      </c>
+      <c r="B81" s="1">
+        <v>39</v>
+      </c>
+      <c r="C81" s="1">
+        <v>5</v>
+      </c>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (63, 39, 5)</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A82">
-        <v>31</v>
-      </c>
-      <c r="B82">
-        <v>48</v>
-      </c>
-      <c r="C82">
-        <v>6</v>
-      </c>
-      <c r="E82" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 48, 6)</v>
+      <c r="A82" s="1">
+        <v>64</v>
+      </c>
+      <c r="B82" s="1">
+        <v>39</v>
+      </c>
+      <c r="C82" s="1">
+        <v>5</v>
+      </c>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (64, 39, 5)</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A83">
-        <v>31</v>
-      </c>
-      <c r="B83">
-        <v>49</v>
-      </c>
-      <c r="C83">
-        <v>6</v>
-      </c>
-      <c r="E83" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 49, 6)</v>
+      <c r="A83" s="1">
+        <v>65</v>
+      </c>
+      <c r="B83" s="1">
+        <v>39</v>
+      </c>
+      <c r="C83" s="1">
+        <v>5</v>
+      </c>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (65, 39, 5)</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A84">
-        <v>31</v>
-      </c>
-      <c r="B84">
-        <v>50</v>
-      </c>
-      <c r="C84">
-        <v>6</v>
-      </c>
-      <c r="E84" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 50, 6)</v>
+      <c r="A84" s="1">
+        <v>66</v>
+      </c>
+      <c r="B84" s="1">
+        <v>39</v>
+      </c>
+      <c r="C84" s="1">
+        <v>5</v>
+      </c>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (66, 39, 5)</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="B85">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C85">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E85" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (32, 40, 6)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (67, 37, 5)</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="B86">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C86">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E86" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (32, 41, 6)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (68, 37, 5)</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="B87">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C87">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E87" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (32, 42, 6)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (69, 37, 5)</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="B88">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C88">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E88" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (33, 40, 6)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (70, 37, 5)</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="B89">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C89">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E89" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (33, 41, 6)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (71, 37, 5)</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="B90">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C90">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E90" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (51, 31, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 40, 6)</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="B91">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C91">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E91" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (52, 31, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 41, 6)</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="B92">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C92">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E92" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (53, 31, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 42, 6)</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="B93">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="C93">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E93" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (54, 31, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 43, 6)</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="B94">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C94">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E94" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (55, 31, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 44, 6)</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="B95">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C95">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E95" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (56, 31, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 45, 6)</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="B96">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C96">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E96" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (57, 31, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 46, 6)</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="B97">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C97">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E97" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (58, 31, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 47, 6)</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="B98">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C98">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E98" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (59, 31, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 48, 6)</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="B99">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="C99">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E99" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (60, 31, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 49, 6)</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="B100">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="C100">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E100" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (61, 32, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (32, 50, 6)</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="B101">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="C101">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E101" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (62, 32, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (32, 51, 6)</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="B102">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="C102">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E102" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (63, 33, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (33, 52, 6)</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="B103">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="C103">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E103" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (64, 33, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (33, 53, 6)</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="B104">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="C104">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E104" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (65, 33, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (33, 54, 6)</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="B105">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="C105">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E105" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (66, 35, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (35, 55, 6)</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="B106">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="C106">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E106" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (67, 34, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (34, 56, 6)</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="B107">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="C107">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E107" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (68, 36, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (36, 57, 6)</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="B108">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="C108">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E108" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (69, 36, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (36, 58, 6)</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="B109">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C109">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E109" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (70, 36, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (36, 59, 6)</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="B110" s="1">
-        <v>38</v>
-      </c>
-      <c r="C110" s="1">
-        <v>5</v>
-      </c>
-      <c r="D110" s="1"/>
-      <c r="E110" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (71, 38, 5)</v>
+        <v>60</v>
+      </c>
+      <c r="C110">
+        <v>6</v>
+      </c>
+      <c r="E110" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (38, 60, 6)</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="B111" s="1">
-        <v>38</v>
-      </c>
-      <c r="C111" s="1">
-        <v>5</v>
-      </c>
-      <c r="D111" s="1"/>
-      <c r="E111" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (72, 38, 5)</v>
+        <v>61</v>
+      </c>
+      <c r="C111">
+        <v>6</v>
+      </c>
+      <c r="E111" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (38, 61, 6)</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="B112" s="1">
-        <v>38</v>
-      </c>
-      <c r="C112" s="1">
-        <v>5</v>
-      </c>
-      <c r="D112" s="1"/>
-      <c r="E112" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (73, 38, 5)</v>
+        <v>62</v>
+      </c>
+      <c r="C112">
+        <v>6</v>
+      </c>
+      <c r="E112" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (38, 62, 6)</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
-        <v>74</v>
+        <v>39</v>
       </c>
       <c r="B113" s="1">
-        <v>39</v>
-      </c>
-      <c r="C113" s="1">
-        <v>5</v>
-      </c>
-      <c r="D113" s="1"/>
-      <c r="E113" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (74, 39, 5)</v>
+        <v>63</v>
+      </c>
+      <c r="C113">
+        <v>6</v>
+      </c>
+      <c r="E113" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (39, 63, 6)</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="B114" s="1">
-        <v>39</v>
-      </c>
-      <c r="C114" s="1">
-        <v>5</v>
-      </c>
-      <c r="D114" s="1"/>
-      <c r="E114" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (75, 39, 5)</v>
+        <v>64</v>
+      </c>
+      <c r="C114">
+        <v>6</v>
+      </c>
+      <c r="E114" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (39, 64, 6)</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="B115" s="1">
-        <v>39</v>
-      </c>
-      <c r="C115" s="1">
-        <v>5</v>
-      </c>
-      <c r="D115" s="1"/>
-      <c r="E115" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (76, 39, 5)</v>
+        <v>65</v>
+      </c>
+      <c r="C115">
+        <v>6</v>
+      </c>
+      <c r="E115" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (39, 65, 6)</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="B116" s="1">
-        <v>39</v>
-      </c>
-      <c r="C116" s="1">
-        <v>5</v>
-      </c>
-      <c r="D116" s="1"/>
-      <c r="E116" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (77, 39, 5)</v>
+        <v>66</v>
+      </c>
+      <c r="C116">
+        <v>6</v>
+      </c>
+      <c r="E116" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (39, 66, 6)</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117">
-        <v>78</v>
+        <v>37</v>
       </c>
       <c r="B117">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="C117">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E117" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (78, 37, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (37, 67, 6)</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="B118">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="C118">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E118" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (79, 37, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (37, 68, 6)</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119">
-        <v>80</v>
+        <v>37</v>
       </c>
       <c r="B119">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="C119">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E119" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (80, 37, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (37, 69, 6)</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120">
-        <v>81</v>
+        <v>37</v>
       </c>
       <c r="B120">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="C120">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E120" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (81, 37, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (37, 70, 6)</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="B121">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="C121">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E121" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (82, 37, 5)</v>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (37, 71, 6)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Split star alleles and allow for multiple results
</commit_message>
<xml_diff>
--- a/MHGR/Data/EAVAttributes/EAVAttributes.xlsx
+++ b/MHGR/Data/EAVAttributes/EAVAttributes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="5840" windowWidth="21360" windowHeight="5900" activeTab="1"/>
+    <workbookView xWindow="-20" yWindow="5840" windowWidth="21360" windowHeight="5900"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes" sheetId="1" r:id="rId1"/>
@@ -281,7 +281,7 @@
     <t>rs397515963</t>
   </si>
   <si>
-    <t>Gene result type</t>
+    <t>Star allele</t>
   </si>
 </sst>
 </file>
@@ -626,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2047,7 +2047,7 @@
       </c>
       <c r="G74" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (73, 'Gene result type', '', NULL, NULL)</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (73, 'Star allele', '', NULL, NULL)</v>
       </c>
     </row>
   </sheetData>
@@ -2060,7 +2060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A123" sqref="A123"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Split SNP alleles for results
</commit_message>
<xml_diff>
--- a/MHGR/Data/EAVAttributes/EAVAttributes.xlsx
+++ b/MHGR/Data/EAVAttributes/EAVAttributes.xlsx
@@ -281,7 +281,7 @@
     <t>rs397515963</t>
   </si>
   <si>
-    <t>Star allele</t>
+    <t>Allele</t>
   </si>
 </sst>
 </file>
@@ -626,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1701,7 +1701,7 @@
         <v>66</v>
       </c>
       <c r="G57" t="str">
-        <f t="shared" ref="G57:G74" si="1">CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A57, ", '", B57, "', '", C74, "', ", IF(D57 = "", "NULL", CONCATENATE("'", D57, "'")), ", ", IF(E57 = "", "NULL", CONCATENATE("'", E57, "'")), ")")</f>
+        <f t="shared" ref="G57" si="1">CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A57, ", '", B57, "', '", C74, "', ", IF(D57 = "", "NULL", CONCATENATE("'", D57, "'")), ", ", IF(E57 = "", "NULL", CONCATENATE("'", E57, "'")), ")")</f>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (56, 'rs1799963', 'short_text', 'rs1799963', 'dbSNP')</v>
       </c>
     </row>
@@ -1721,9 +1721,9 @@
       <c r="E58" t="s">
         <v>66</v>
       </c>
-      <c r="G58" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (57, 'rs121913626', '', 'rs121913626', 'dbSNP')</v>
+      <c r="G58" t="e">
+        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A58, ", '", B58, "', '",#REF!, "', ", IF(D58 = "", "NULL", CONCATENATE("'", D58, "'")), ", ", IF(E58 = "", "NULL", CONCATENATE("'", E58, "'")), ")")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
@@ -1743,7 +1743,7 @@
         <v>66</v>
       </c>
       <c r="G59" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A59, ", '", B59, "', '", C75, "', ", IF(D59 = "", "NULL", CONCATENATE("'", D59, "'")), ", ", IF(E59 = "", "NULL", CONCATENATE("'", E59, "'")), ")")</f>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (58, 'rs3218713', '', 'rs3218713', 'dbSNP')</v>
       </c>
     </row>
@@ -1764,7 +1764,7 @@
         <v>66</v>
       </c>
       <c r="G60" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A60, ", '", B60, "', '", C76, "', ", IF(D60 = "", "NULL", CONCATENATE("'", D60, "'")), ", ", IF(E60 = "", "NULL", CONCATENATE("'", E60, "'")), ")")</f>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (59, 'rs3218714', '', 'rs3218714', 'dbSNP')</v>
       </c>
     </row>
@@ -1785,7 +1785,7 @@
         <v>66</v>
       </c>
       <c r="G61" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A61, ", '", B61, "', '", C77, "', ", IF(D61 = "", "NULL", CONCATENATE("'", D61, "'")), ", ", IF(E61 = "", "NULL", CONCATENATE("'", E61, "'")), ")")</f>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (60, 'rs121964855', '', 'rs121964855', 'dbSNP')</v>
       </c>
     </row>
@@ -1806,7 +1806,7 @@
         <v>66</v>
       </c>
       <c r="G62" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A62, ", '", B62, "', '", C78, "', ", IF(D62 = "", "NULL", CONCATENATE("'", D62, "'")), ", ", IF(E62 = "", "NULL", CONCATENATE("'", E62, "'")), ")")</f>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (61, 'rs121964856', '', 'rs121964856', 'dbSNP')</v>
       </c>
     </row>
@@ -1827,7 +1827,7 @@
         <v>66</v>
       </c>
       <c r="G63" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A63, ", '", B63, "', '", C79, "', ", IF(D63 = "", "NULL", CONCATENATE("'", D63, "'")), ", ", IF(E63 = "", "NULL", CONCATENATE("'", E63, "'")), ")")</f>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (62, 'rs121964857', '', 'rs121964857', 'dbSNP')</v>
       </c>
     </row>
@@ -1848,7 +1848,7 @@
         <v>66</v>
       </c>
       <c r="G64" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A64, ", '", B64, "', '", C80, "', ", IF(D64 = "", "NULL", CONCATENATE("'", D64, "'")), ", ", IF(E64 = "", "NULL", CONCATENATE("'", E64, "'")), ")")</f>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (63, 'rs28934269', '', 'rs28934269', 'dbSNP')</v>
       </c>
     </row>
@@ -1869,7 +1869,7 @@
         <v>66</v>
       </c>
       <c r="G65" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A65, ", '", B65, "', '", C81, "', ", IF(D65 = "", "NULL", CONCATENATE("'", D65, "'")), ", ", IF(E65 = "", "NULL", CONCATENATE("'", E65, "'")), ")")</f>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (64, 'rs28934270', '', 'rs28934270', 'dbSNP')</v>
       </c>
     </row>
@@ -1890,7 +1890,7 @@
         <v>66</v>
       </c>
       <c r="G66" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A66, ", '", B66, "', '", C82, "', ", IF(D66 = "", "NULL", CONCATENATE("'", D66, "'")), ", ", IF(E66 = "", "NULL", CONCATENATE("'", E66, "'")), ")")</f>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (65, 'rs727504290', '', 'rs727504290', 'dbSNP')</v>
       </c>
     </row>
@@ -1911,7 +1911,7 @@
         <v>66</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A67, ", '", B67, "', '", C83, "', ", IF(D67 = "", "NULL", CONCATENATE("'", D67, "'")), ", ", IF(E67 = "", "NULL", CONCATENATE("'", E67, "'")), ")")</f>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (66, 'rs104894504', '', 'rs104894504', 'dbSNP')</v>
       </c>
     </row>
@@ -1932,7 +1932,7 @@
         <v>66</v>
       </c>
       <c r="G68" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A68, ", '", B68, "', '", C84, "', ", IF(D68 = "", "NULL", CONCATENATE("'", D68, "'")), ", ", IF(E68 = "", "NULL", CONCATENATE("'", E68, "'")), ")")</f>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (67, 'rs375882485', '', 'rs375882485', 'dbSNP')</v>
       </c>
     </row>
@@ -1953,7 +1953,7 @@
         <v>66</v>
       </c>
       <c r="G69" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A69, ", '", B69, "', '", C85, "', ", IF(D69 = "", "NULL", CONCATENATE("'", D69, "'")), ", ", IF(E69 = "", "NULL", CONCATENATE("'", E69, "'")), ")")</f>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (68, 'rs397516083', '', 'rs397516083', 'dbSNP')</v>
       </c>
     </row>
@@ -1974,7 +1974,7 @@
         <v>66</v>
       </c>
       <c r="G70" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A70, ", '", B70, "', '", C86, "', ", IF(D70 = "", "NULL", CONCATENATE("'", D70, "'")), ", ", IF(E70 = "", "NULL", CONCATENATE("'", E70, "'")), ")")</f>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (69, 'rs397515937', '', 'rs397515937', 'dbSNP')</v>
       </c>
     </row>
@@ -1995,7 +1995,7 @@
         <v>66</v>
       </c>
       <c r="G71" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A71, ", '", B71, "', '", C87, "', ", IF(D71 = "", "NULL", CONCATENATE("'", D71, "'")), ", ", IF(E71 = "", "NULL", CONCATENATE("'", E71, "'")), ")")</f>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (70, 'rs397516074', '', 'rs397516074', 'dbSNP')</v>
       </c>
     </row>
@@ -2016,7 +2016,7 @@
         <v>66</v>
       </c>
       <c r="G72" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A72, ", '", B72, "', '", C88, "', ", IF(D72 = "", "NULL", CONCATENATE("'", D72, "'")), ", ", IF(E72 = "", "NULL", CONCATENATE("'", E72, "'")), ")")</f>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (71, 'rs397515963', '', 'rs397515963', 'dbSNP')</v>
       </c>
     </row>
@@ -2031,7 +2031,7 @@
         <v>68</v>
       </c>
       <c r="G73" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A73, ", '", B73, "', '", C89, "', ", IF(D73 = "", "NULL", CONCATENATE("'", D73, "'")), ", ", IF(E73 = "", "NULL", CONCATENATE("'", E73, "'")), ")")</f>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (72, 'Resulted on', '', NULL, NULL)</v>
       </c>
     </row>
@@ -2046,8 +2046,8 @@
         <v>61</v>
       </c>
       <c r="G74" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (73, 'Star allele', '', NULL, NULL)</v>
+        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A74, ", '", B74, "', '", C90, "', ", IF(D74 = "", "NULL", CONCATENATE("'", D74, "'")), ", ", IF(E74 = "", "NULL", CONCATENATE("'", E74, "'")), ")")</f>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (73, 'Allele', '', NULL, NULL)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP loading GVFs for EAV schema
</commit_message>
<xml_diff>
--- a/MHGR/Data/EAVAttributes/EAVAttributes.xlsx
+++ b/MHGR/Data/EAVAttributes/EAVAttributes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="120">
   <si>
     <t>Name</t>
   </si>
@@ -282,6 +282,105 @@
   </si>
   <si>
     <t>Allele</t>
+  </si>
+  <si>
+    <t>Genomic Variant Format result</t>
+  </si>
+  <si>
+    <t>GVF Version</t>
+  </si>
+  <si>
+    <t>GFF Version</t>
+  </si>
+  <si>
+    <t>File Version</t>
+  </si>
+  <si>
+    <t>Source method</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Source type</t>
+  </si>
+  <si>
+    <t>Dbxref</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>Technology platform</t>
+  </si>
+  <si>
+    <t>Platform class</t>
+  </si>
+  <si>
+    <t>Platform name</t>
+  </si>
+  <si>
+    <t>Read type</t>
+  </si>
+  <si>
+    <t>Read length</t>
+  </si>
+  <si>
+    <t>Read pair span</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>Average coverage</t>
+  </si>
+  <si>
+    <t>Feature ontology</t>
+  </si>
+  <si>
+    <t>Genome build</t>
+  </si>
+  <si>
+    <t>Sequence region</t>
+  </si>
+  <si>
+    <t>Chromosome</t>
+  </si>
+  <si>
+    <t>Start position</t>
+  </si>
+  <si>
+    <t>End position</t>
+  </si>
+  <si>
+    <t>source-method</t>
+  </si>
+  <si>
+    <t>technology-platform</t>
+  </si>
+  <si>
+    <t>feature-ontology</t>
+  </si>
+  <si>
+    <t>genome-build</t>
+  </si>
+  <si>
+    <t>sequence-region</t>
+  </si>
+  <si>
+    <t>GVF</t>
+  </si>
+  <si>
+    <t>gvf-version</t>
+  </si>
+  <si>
+    <t>gff-version</t>
+  </si>
+  <si>
+    <t>file-version</t>
   </si>
 </sst>
 </file>
@@ -624,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:G96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G96" sqref="G2:G96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -681,7 +780,7 @@
         <v>2</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G54" si="0">CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A3, ", '", B3, "', '", C3, "', ", IF(D3 = "", "NULL", CONCATENATE("'", D3, "'")), ", ", IF(E3 = "", "NULL", CONCATENATE("'", E3, "'")), ")")</f>
+        <f t="shared" ref="G3:G66" si="0">CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A3, ", '", B3, "', '", C3, "', ", IF(D3 = "", "NULL", CONCATENATE("'", D3, "'")), ", ", IF(E3 = "", "NULL", CONCATENATE("'", E3, "'")), ")")</f>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (2, 'Is a', 'binary', NULL, NULL)</v>
       </c>
     </row>
@@ -1659,7 +1758,7 @@
         <v>66</v>
       </c>
       <c r="G55" t="str">
-        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A55, ", '", B55, "', '", C72, "', ", IF(D55 = "", "NULL", CONCATENATE("'", D55, "'")), ", ", IF(E55 = "", "NULL", CONCATENATE("'", E55, "'")), ")")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (54, 'rs8050894', 'short_text', 'rs8050894', 'dbSNP')</v>
       </c>
     </row>
@@ -1680,8 +1779,8 @@
         <v>66</v>
       </c>
       <c r="G56" t="str">
-        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A56, ", '", B56, "', '", C73, "', ", IF(D56 = "", "NULL", CONCATENATE("'", D56, "'")), ", ", IF(E56 = "", "NULL", CONCATENATE("'", E56, "'")), ")")</f>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (55, 'rs6025', 'date_time', 'rs6025', 'dbSNP')</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (55, 'rs6025', 'short_text', 'rs6025', 'dbSNP')</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
@@ -1701,7 +1800,7 @@
         <v>66</v>
       </c>
       <c r="G57" t="str">
-        <f t="shared" ref="G57" si="1">CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A57, ", '", B57, "', '", C74, "', ", IF(D57 = "", "NULL", CONCATENATE("'", D57, "'")), ", ", IF(E57 = "", "NULL", CONCATENATE("'", E57, "'")), ")")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (56, 'rs1799963', 'short_text', 'rs1799963', 'dbSNP')</v>
       </c>
     </row>
@@ -1721,9 +1820,9 @@
       <c r="E58" t="s">
         <v>66</v>
       </c>
-      <c r="G58" t="e">
-        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A58, ", '", B58, "', '",#REF!, "', ", IF(D58 = "", "NULL", CONCATENATE("'", D58, "'")), ", ", IF(E58 = "", "NULL", CONCATENATE("'", E58, "'")), ")")</f>
-        <v>#REF!</v>
+      <c r="G58" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (57, 'rs121913626', 'short_text', 'rs121913626', 'dbSNP')</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
@@ -1743,8 +1842,8 @@
         <v>66</v>
       </c>
       <c r="G59" t="str">
-        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A59, ", '", B59, "', '", C75, "', ", IF(D59 = "", "NULL", CONCATENATE("'", D59, "'")), ", ", IF(E59 = "", "NULL", CONCATENATE("'", E59, "'")), ")")</f>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (58, 'rs3218713', '', 'rs3218713', 'dbSNP')</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (58, 'rs3218713', 'short_text', 'rs3218713', 'dbSNP')</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
@@ -1764,8 +1863,8 @@
         <v>66</v>
       </c>
       <c r="G60" t="str">
-        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A60, ", '", B60, "', '", C76, "', ", IF(D60 = "", "NULL", CONCATENATE("'", D60, "'")), ", ", IF(E60 = "", "NULL", CONCATENATE("'", E60, "'")), ")")</f>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (59, 'rs3218714', '', 'rs3218714', 'dbSNP')</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (59, 'rs3218714', 'short_text', 'rs3218714', 'dbSNP')</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
@@ -1785,8 +1884,8 @@
         <v>66</v>
       </c>
       <c r="G61" t="str">
-        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A61, ", '", B61, "', '", C77, "', ", IF(D61 = "", "NULL", CONCATENATE("'", D61, "'")), ", ", IF(E61 = "", "NULL", CONCATENATE("'", E61, "'")), ")")</f>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (60, 'rs121964855', '', 'rs121964855', 'dbSNP')</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (60, 'rs121964855', 'short_text', 'rs121964855', 'dbSNP')</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
@@ -1806,8 +1905,8 @@
         <v>66</v>
       </c>
       <c r="G62" t="str">
-        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A62, ", '", B62, "', '", C78, "', ", IF(D62 = "", "NULL", CONCATENATE("'", D62, "'")), ", ", IF(E62 = "", "NULL", CONCATENATE("'", E62, "'")), ")")</f>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (61, 'rs121964856', '', 'rs121964856', 'dbSNP')</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (61, 'rs121964856', 'short_text', 'rs121964856', 'dbSNP')</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
@@ -1827,8 +1926,8 @@
         <v>66</v>
       </c>
       <c r="G63" t="str">
-        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A63, ", '", B63, "', '", C79, "', ", IF(D63 = "", "NULL", CONCATENATE("'", D63, "'")), ", ", IF(E63 = "", "NULL", CONCATENATE("'", E63, "'")), ")")</f>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (62, 'rs121964857', '', 'rs121964857', 'dbSNP')</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (62, 'rs121964857', 'short_text', 'rs121964857', 'dbSNP')</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
@@ -1848,8 +1947,8 @@
         <v>66</v>
       </c>
       <c r="G64" t="str">
-        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A64, ", '", B64, "', '", C80, "', ", IF(D64 = "", "NULL", CONCATENATE("'", D64, "'")), ", ", IF(E64 = "", "NULL", CONCATENATE("'", E64, "'")), ")")</f>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (63, 'rs28934269', '', 'rs28934269', 'dbSNP')</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (63, 'rs28934269', 'short_text', 'rs28934269', 'dbSNP')</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
@@ -1869,8 +1968,8 @@
         <v>66</v>
       </c>
       <c r="G65" t="str">
-        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A65, ", '", B65, "', '", C81, "', ", IF(D65 = "", "NULL", CONCATENATE("'", D65, "'")), ", ", IF(E65 = "", "NULL", CONCATENATE("'", E65, "'")), ")")</f>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (64, 'rs28934270', '', 'rs28934270', 'dbSNP')</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (64, 'rs28934270', 'short_text', 'rs28934270', 'dbSNP')</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
@@ -1890,8 +1989,8 @@
         <v>66</v>
       </c>
       <c r="G66" t="str">
-        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A66, ", '", B66, "', '", C82, "', ", IF(D66 = "", "NULL", CONCATENATE("'", D66, "'")), ", ", IF(E66 = "", "NULL", CONCATENATE("'", E66, "'")), ")")</f>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (65, 'rs727504290', '', 'rs727504290', 'dbSNP')</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (65, 'rs727504290', 'short_text', 'rs727504290', 'dbSNP')</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
@@ -1911,8 +2010,8 @@
         <v>66</v>
       </c>
       <c r="G67" t="str">
-        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A67, ", '", B67, "', '", C83, "', ", IF(D67 = "", "NULL", CONCATENATE("'", D67, "'")), ", ", IF(E67 = "", "NULL", CONCATENATE("'", E67, "'")), ")")</f>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (66, 'rs104894504', '', 'rs104894504', 'dbSNP')</v>
+        <f t="shared" ref="G67:G96" si="1">CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A67, ", '", B67, "', '", C67, "', ", IF(D67 = "", "NULL", CONCATENATE("'", D67, "'")), ", ", IF(E67 = "", "NULL", CONCATENATE("'", E67, "'")), ")")</f>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (66, 'rs104894504', 'short_text', 'rs104894504', 'dbSNP')</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
@@ -1932,8 +2031,8 @@
         <v>66</v>
       </c>
       <c r="G68" t="str">
-        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A68, ", '", B68, "', '", C84, "', ", IF(D68 = "", "NULL", CONCATENATE("'", D68, "'")), ", ", IF(E68 = "", "NULL", CONCATENATE("'", E68, "'")), ")")</f>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (67, 'rs375882485', '', 'rs375882485', 'dbSNP')</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (67, 'rs375882485', 'short_text', 'rs375882485', 'dbSNP')</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
@@ -1953,8 +2052,8 @@
         <v>66</v>
       </c>
       <c r="G69" t="str">
-        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A69, ", '", B69, "', '", C85, "', ", IF(D69 = "", "NULL", CONCATENATE("'", D69, "'")), ", ", IF(E69 = "", "NULL", CONCATENATE("'", E69, "'")), ")")</f>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (68, 'rs397516083', '', 'rs397516083', 'dbSNP')</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (68, 'rs397516083', 'short_text', 'rs397516083', 'dbSNP')</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
@@ -1974,8 +2073,8 @@
         <v>66</v>
       </c>
       <c r="G70" t="str">
-        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A70, ", '", B70, "', '", C86, "', ", IF(D70 = "", "NULL", CONCATENATE("'", D70, "'")), ", ", IF(E70 = "", "NULL", CONCATENATE("'", E70, "'")), ")")</f>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (69, 'rs397515937', '', 'rs397515937', 'dbSNP')</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (69, 'rs397515937', 'short_text', 'rs397515937', 'dbSNP')</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
@@ -1995,8 +2094,8 @@
         <v>66</v>
       </c>
       <c r="G71" t="str">
-        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A71, ", '", B71, "', '", C87, "', ", IF(D71 = "", "NULL", CONCATENATE("'", D71, "'")), ", ", IF(E71 = "", "NULL", CONCATENATE("'", E71, "'")), ")")</f>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (70, 'rs397516074', '', 'rs397516074', 'dbSNP')</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (70, 'rs397516074', 'short_text', 'rs397516074', 'dbSNP')</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
@@ -2016,8 +2115,8 @@
         <v>66</v>
       </c>
       <c r="G72" t="str">
-        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A72, ", '", B72, "', '", C88, "', ", IF(D72 = "", "NULL", CONCATENATE("'", D72, "'")), ", ", IF(E72 = "", "NULL", CONCATENATE("'", E72, "'")), ")")</f>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (71, 'rs397515963', '', 'rs397515963', 'dbSNP')</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (71, 'rs397515963', 'short_text', 'rs397515963', 'dbSNP')</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
@@ -2031,8 +2130,8 @@
         <v>68</v>
       </c>
       <c r="G73" t="str">
-        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A73, ", '", B73, "', '", C89, "', ", IF(D73 = "", "NULL", CONCATENATE("'", D73, "'")), ", ", IF(E73 = "", "NULL", CONCATENATE("'", E73, "'")), ")")</f>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (72, 'Resulted on', '', NULL, NULL)</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (72, 'Resulted on', 'date_time', NULL, NULL)</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
@@ -2046,8 +2145,386 @@
         <v>61</v>
       </c>
       <c r="G74" t="str">
-        <f>CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A74, ", '", B74, "', '", C90, "', ", IF(D74 = "", "NULL", CONCATENATE("'", D74, "'")), ", ", IF(E74 = "", "NULL", CONCATENATE("'", E74, "'")), ")")</f>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (73, 'Allele', '', NULL, NULL)</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (73, 'Allele', 'short_text', NULL, NULL)</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>87</v>
+      </c>
+      <c r="C75" t="s">
+        <v>2</v>
+      </c>
+      <c r="G75" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (74, 'Genomic Variant Format result', 'binary', NULL, NULL)</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>88</v>
+      </c>
+      <c r="C76" t="s">
+        <v>61</v>
+      </c>
+      <c r="D76" t="s">
+        <v>117</v>
+      </c>
+      <c r="E76" t="s">
+        <v>116</v>
+      </c>
+      <c r="G76" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (75, 'GVF Version', 'short_text', 'gvf-version', 'GVF')</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>89</v>
+      </c>
+      <c r="C77" t="s">
+        <v>61</v>
+      </c>
+      <c r="D77" t="s">
+        <v>118</v>
+      </c>
+      <c r="E77" t="s">
+        <v>116</v>
+      </c>
+      <c r="G77" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (76, 'GFF Version', 'short_text', 'gff-version', 'GVF')</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>90</v>
+      </c>
+      <c r="C78" t="s">
+        <v>61</v>
+      </c>
+      <c r="D78" t="s">
+        <v>119</v>
+      </c>
+      <c r="E78" t="s">
+        <v>116</v>
+      </c>
+      <c r="G78" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (77, 'File Version', 'short_text', 'file-version', 'GVF')</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>91</v>
+      </c>
+      <c r="C79" t="s">
+        <v>2</v>
+      </c>
+      <c r="D79" t="s">
+        <v>111</v>
+      </c>
+      <c r="E79" t="s">
+        <v>116</v>
+      </c>
+      <c r="G79" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (78, 'Source method', 'binary', 'source-method', 'GVF')</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>92</v>
+      </c>
+      <c r="C80" t="s">
+        <v>61</v>
+      </c>
+      <c r="G80" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (79, 'Source', 'short_text', NULL, NULL)</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>93</v>
+      </c>
+      <c r="C81" t="s">
+        <v>61</v>
+      </c>
+      <c r="G81" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (80, 'Source type', 'short_text', NULL, NULL)</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>94</v>
+      </c>
+      <c r="C82" t="s">
+        <v>61</v>
+      </c>
+      <c r="G82" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (81, 'Dbxref', 'short_text', NULL, NULL)</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>95</v>
+      </c>
+      <c r="C83" t="s">
+        <v>96</v>
+      </c>
+      <c r="G83" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (82, 'Comment', 'text', NULL, NULL)</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>97</v>
+      </c>
+      <c r="C84" t="s">
+        <v>2</v>
+      </c>
+      <c r="D84" t="s">
+        <v>112</v>
+      </c>
+      <c r="E84" t="s">
+        <v>116</v>
+      </c>
+      <c r="G84" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (83, 'Technology platform', 'binary', 'technology-platform', 'GVF')</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>98</v>
+      </c>
+      <c r="C85" t="s">
+        <v>61</v>
+      </c>
+      <c r="G85" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (84, 'Platform class', 'short_text', NULL, NULL)</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>99</v>
+      </c>
+      <c r="C86" t="s">
+        <v>61</v>
+      </c>
+      <c r="G86" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (85, 'Platform name', 'short_text', NULL, NULL)</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>100</v>
+      </c>
+      <c r="C87" t="s">
+        <v>61</v>
+      </c>
+      <c r="G87" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (86, 'Read type', 'short_text', NULL, NULL)</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>101</v>
+      </c>
+      <c r="C88" t="s">
+        <v>103</v>
+      </c>
+      <c r="G88" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (87, 'Read length', 'int', NULL, NULL)</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>102</v>
+      </c>
+      <c r="C89" t="s">
+        <v>103</v>
+      </c>
+      <c r="G89" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (88, 'Read pair span', 'int', NULL, NULL)</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>104</v>
+      </c>
+      <c r="C90" t="s">
+        <v>103</v>
+      </c>
+      <c r="G90" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (89, 'Average coverage', 'int', NULL, NULL)</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>105</v>
+      </c>
+      <c r="C91" t="s">
+        <v>61</v>
+      </c>
+      <c r="D91" t="s">
+        <v>113</v>
+      </c>
+      <c r="E91" t="s">
+        <v>116</v>
+      </c>
+      <c r="G91" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (90, 'Feature ontology', 'short_text', 'feature-ontology', 'GVF')</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>106</v>
+      </c>
+      <c r="C92" t="s">
+        <v>61</v>
+      </c>
+      <c r="D92" t="s">
+        <v>114</v>
+      </c>
+      <c r="E92" t="s">
+        <v>116</v>
+      </c>
+      <c r="G92" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (91, 'Genome build', 'short_text', 'genome-build', 'GVF')</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>107</v>
+      </c>
+      <c r="C93" t="s">
+        <v>2</v>
+      </c>
+      <c r="D93" t="s">
+        <v>115</v>
+      </c>
+      <c r="E93" t="s">
+        <v>116</v>
+      </c>
+      <c r="G93" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (92, 'Sequence region', 'binary', 'sequence-region', 'GVF')</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>108</v>
+      </c>
+      <c r="C94" t="s">
+        <v>103</v>
+      </c>
+      <c r="G94" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (93, 'Chromosome', 'int', NULL, NULL)</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>109</v>
+      </c>
+      <c r="C95" t="s">
+        <v>103</v>
+      </c>
+      <c r="G95" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (94, 'Start position', 'int', NULL, NULL)</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>110</v>
+      </c>
+      <c r="C96" t="s">
+        <v>103</v>
+      </c>
+      <c r="G96" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (95, 'End position', 'int', NULL, NULL)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GVF loader for EAV schema
</commit_message>
<xml_diff>
--- a/MHGR/Data/EAVAttributes/EAVAttributes.xlsx
+++ b/MHGR/Data/EAVAttributes/EAVAttributes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="135">
   <si>
     <t>Name</t>
   </si>
@@ -302,9 +302,6 @@
     <t>Source</t>
   </si>
   <si>
-    <t>Source type</t>
-  </si>
-  <si>
     <t>Dbxref</t>
   </si>
   <si>
@@ -381,6 +378,54 @@
   </si>
   <si>
     <t>file-version</t>
+  </si>
+  <si>
+    <t>Platform_class</t>
+  </si>
+  <si>
+    <t>Platform_name</t>
+  </si>
+  <si>
+    <t>Read_type</t>
+  </si>
+  <si>
+    <t>Read_length</t>
+  </si>
+  <si>
+    <t>Average_coverage</t>
+  </si>
+  <si>
+    <t>Read_pair_span</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Genomic Variant Format feature</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Strand</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Reference sequence</t>
+  </si>
+  <si>
+    <t>Reference_seq</t>
+  </si>
+  <si>
+    <t>Variant_reads</t>
+  </si>
+  <si>
+    <t>Genotype</t>
+  </si>
+  <si>
+    <t>Variant reads</t>
   </si>
 </sst>
 </file>
@@ -723,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G96"/>
+  <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G96" sqref="G2:G96"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2010,7 +2055,7 @@
         <v>66</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" ref="G67:G96" si="1">CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A67, ", '", B67, "', '", C67, "', ", IF(D67 = "", "NULL", CONCATENATE("'", D67, "'")), ", ", IF(E67 = "", "NULL", CONCATENATE("'", E67, "'")), ")")</f>
+        <f t="shared" ref="G67:G103" si="1">CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A67, ", '", B67, "', '", C67, "', ", IF(D67 = "", "NULL", CONCATENATE("'", D67, "'")), ", ", IF(E67 = "", "NULL", CONCATENATE("'", E67, "'")), ")")</f>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (66, 'rs104894504', 'short_text', 'rs104894504', 'dbSNP')</v>
       </c>
     </row>
@@ -2175,10 +2220,10 @@
         <v>61</v>
       </c>
       <c r="D76" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E76" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G76" t="str">
         <f t="shared" si="1"/>
@@ -2196,10 +2241,10 @@
         <v>61</v>
       </c>
       <c r="D77" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E77" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G77" t="str">
         <f t="shared" si="1"/>
@@ -2217,10 +2262,10 @@
         <v>61</v>
       </c>
       <c r="D78" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E78" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G78" t="str">
         <f t="shared" si="1"/>
@@ -2238,10 +2283,10 @@
         <v>2</v>
       </c>
       <c r="D79" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E79" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G79" t="str">
         <f t="shared" si="1"/>
@@ -2258,9 +2303,15 @@
       <c r="C80" t="s">
         <v>61</v>
       </c>
+      <c r="D80" t="s">
+        <v>92</v>
+      </c>
+      <c r="E80" t="s">
+        <v>115</v>
+      </c>
       <c r="G80" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (79, 'Source', 'short_text', NULL, NULL)</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (79, 'Source', 'short_text', 'Source', 'GVF')</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
@@ -2268,14 +2319,20 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="C81" t="s">
         <v>61</v>
       </c>
+      <c r="D81" t="s">
+        <v>125</v>
+      </c>
+      <c r="E81" t="s">
+        <v>115</v>
+      </c>
       <c r="G81" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (80, 'Source type', 'short_text', NULL, NULL)</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (80, 'Type', 'short_text', 'Type', 'GVF')</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
@@ -2283,14 +2340,20 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C82" t="s">
         <v>61</v>
       </c>
+      <c r="D82" t="s">
+        <v>93</v>
+      </c>
+      <c r="E82" t="s">
+        <v>115</v>
+      </c>
       <c r="G82" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (81, 'Dbxref', 'short_text', NULL, NULL)</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (81, 'Dbxref', 'short_text', 'Dbxref', 'GVF')</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
@@ -2298,14 +2361,20 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
+        <v>94</v>
+      </c>
+      <c r="C83" t="s">
         <v>95</v>
       </c>
-      <c r="C83" t="s">
-        <v>96</v>
+      <c r="D83" t="s">
+        <v>94</v>
+      </c>
+      <c r="E83" t="s">
+        <v>115</v>
       </c>
       <c r="G83" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (82, 'Comment', 'text', NULL, NULL)</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (82, 'Comment', 'text', 'Comment', 'GVF')</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
@@ -2313,16 +2382,16 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C84" t="s">
         <v>2</v>
       </c>
       <c r="D84" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E84" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G84" t="str">
         <f t="shared" si="1"/>
@@ -2334,14 +2403,20 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C85" t="s">
         <v>61</v>
       </c>
+      <c r="D85" t="s">
+        <v>119</v>
+      </c>
+      <c r="E85" t="s">
+        <v>115</v>
+      </c>
       <c r="G85" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (84, 'Platform class', 'short_text', NULL, NULL)</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (84, 'Platform class', 'short_text', 'Platform_class', 'GVF')</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
@@ -2349,14 +2424,20 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C86" t="s">
         <v>61</v>
       </c>
+      <c r="D86" t="s">
+        <v>120</v>
+      </c>
+      <c r="E86" t="s">
+        <v>115</v>
+      </c>
       <c r="G86" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (85, 'Platform name', 'short_text', NULL, NULL)</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (85, 'Platform name', 'short_text', 'Platform_name', 'GVF')</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
@@ -2364,14 +2445,20 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C87" t="s">
         <v>61</v>
       </c>
+      <c r="D87" t="s">
+        <v>121</v>
+      </c>
+      <c r="E87" t="s">
+        <v>115</v>
+      </c>
       <c r="G87" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (86, 'Read type', 'short_text', NULL, NULL)</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (86, 'Read type', 'short_text', 'Read_type', 'GVF')</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
@@ -2379,14 +2466,20 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C88" t="s">
-        <v>103</v>
+        <v>102</v>
+      </c>
+      <c r="D88" t="s">
+        <v>122</v>
+      </c>
+      <c r="E88" t="s">
+        <v>115</v>
       </c>
       <c r="G88" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (87, 'Read length', 'int', NULL, NULL)</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (87, 'Read length', 'int', 'Read_length', 'GVF')</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
@@ -2394,14 +2487,20 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C89" t="s">
-        <v>103</v>
+        <v>61</v>
+      </c>
+      <c r="D89" t="s">
+        <v>124</v>
+      </c>
+      <c r="E89" t="s">
+        <v>115</v>
       </c>
       <c r="G89" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (88, 'Read pair span', 'int', NULL, NULL)</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (88, 'Read pair span', 'short_text', 'Read_pair_span', 'GVF')</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
@@ -2409,14 +2508,20 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C90" t="s">
-        <v>103</v>
+        <v>102</v>
+      </c>
+      <c r="D90" t="s">
+        <v>123</v>
+      </c>
+      <c r="E90" t="s">
+        <v>115</v>
       </c>
       <c r="G90" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (89, 'Average coverage', 'int', NULL, NULL)</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (89, 'Average coverage', 'int', 'Average_coverage', 'GVF')</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
@@ -2424,16 +2529,16 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C91" t="s">
         <v>61</v>
       </c>
       <c r="D91" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E91" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G91" t="str">
         <f t="shared" si="1"/>
@@ -2445,16 +2550,16 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C92" t="s">
         <v>61</v>
       </c>
       <c r="D92" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E92" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G92" t="str">
         <f t="shared" si="1"/>
@@ -2466,16 +2571,16 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C93" t="s">
         <v>2</v>
       </c>
       <c r="D93" t="s">
+        <v>114</v>
+      </c>
+      <c r="E93" t="s">
         <v>115</v>
-      </c>
-      <c r="E93" t="s">
-        <v>116</v>
       </c>
       <c r="G93" t="str">
         <f t="shared" si="1"/>
@@ -2487,14 +2592,20 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C94" t="s">
-        <v>103</v>
+        <v>61</v>
+      </c>
+      <c r="D94" t="s">
+        <v>107</v>
+      </c>
+      <c r="E94" t="s">
+        <v>115</v>
       </c>
       <c r="G94" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (93, 'Chromosome', 'int', NULL, NULL)</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (93, 'Chromosome', 'short_text', 'Chromosome', 'GVF')</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.35">
@@ -2502,14 +2613,20 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C95" t="s">
-        <v>103</v>
+        <v>102</v>
+      </c>
+      <c r="D95" t="s">
+        <v>108</v>
+      </c>
+      <c r="E95" t="s">
+        <v>115</v>
       </c>
       <c r="G95" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (94, 'Start position', 'int', NULL, NULL)</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (94, 'Start position', 'int', 'Start position', 'GVF')</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.35">
@@ -2517,14 +2634,161 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C96" t="s">
-        <v>103</v>
+        <v>102</v>
+      </c>
+      <c r="D96" t="s">
+        <v>109</v>
+      </c>
+      <c r="E96" t="s">
+        <v>115</v>
       </c>
       <c r="G96" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (95, 'End position', 'int', NULL, NULL)</v>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (95, 'End position', 'int', 'End position', 'GVF')</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>126</v>
+      </c>
+      <c r="C97" t="s">
+        <v>2</v>
+      </c>
+      <c r="G97" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (96, 'Genomic Variant Format feature', 'binary', NULL, NULL)</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>127</v>
+      </c>
+      <c r="C98" t="s">
+        <v>61</v>
+      </c>
+      <c r="D98" t="s">
+        <v>127</v>
+      </c>
+      <c r="E98" t="s">
+        <v>115</v>
+      </c>
+      <c r="G98" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (97, 'Score', 'short_text', 'Score', 'GVF')</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>128</v>
+      </c>
+      <c r="C99" t="s">
+        <v>61</v>
+      </c>
+      <c r="D99" t="s">
+        <v>128</v>
+      </c>
+      <c r="E99" t="s">
+        <v>115</v>
+      </c>
+      <c r="G99" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (98, 'Strand', 'short_text', 'Strand', 'GVF')</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>129</v>
+      </c>
+      <c r="C100" t="s">
+        <v>61</v>
+      </c>
+      <c r="D100" t="s">
+        <v>129</v>
+      </c>
+      <c r="E100" t="s">
+        <v>115</v>
+      </c>
+      <c r="G100" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (99, 'Phase', 'short_text', 'Phase', 'GVF')</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>130</v>
+      </c>
+      <c r="C101" t="s">
+        <v>61</v>
+      </c>
+      <c r="D101" t="s">
+        <v>131</v>
+      </c>
+      <c r="E101" t="s">
+        <v>115</v>
+      </c>
+      <c r="G101" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (100, 'Reference sequence', 'short_text', 'Reference_seq', 'GVF')</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
+        <v>134</v>
+      </c>
+      <c r="C102" t="s">
+        <v>61</v>
+      </c>
+      <c r="D102" t="s">
+        <v>132</v>
+      </c>
+      <c r="E102" t="s">
+        <v>115</v>
+      </c>
+      <c r="G102" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (101, 'Variant reads', 'short_text', 'Variant_reads', 'GVF')</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>133</v>
+      </c>
+      <c r="C103" t="s">
+        <v>61</v>
+      </c>
+      <c r="D103" t="s">
+        <v>133</v>
+      </c>
+      <c r="E103" t="s">
+        <v>115</v>
+      </c>
+      <c r="G103" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (102, 'Genotype', 'short_text', 'Genotype', 'GVF')</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP VCF loader for EAV schema
</commit_message>
<xml_diff>
--- a/MHGR/Data/EAVAttributes/EAVAttributes.xlsx
+++ b/MHGR/Data/EAVAttributes/EAVAttributes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="151">
   <si>
     <t>Name</t>
   </si>
@@ -426,6 +426,54 @@
   </si>
   <si>
     <t>Variant reads</t>
+  </si>
+  <si>
+    <t>Variant Call Format result</t>
+  </si>
+  <si>
+    <t>File Format</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>fileFormat</t>
+  </si>
+  <si>
+    <t>VCF</t>
+  </si>
+  <si>
+    <t>Phasing</t>
+  </si>
+  <si>
+    <t>phasing</t>
+  </si>
+  <si>
+    <t>Information</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>INFO</t>
+  </si>
+  <si>
+    <t>FILTER</t>
+  </si>
+  <si>
+    <t>FORMAT</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
@@ -768,10 +816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G103"/>
+  <dimension ref="A1:G114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G112" sqref="G112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2055,7 +2103,7 @@
         <v>66</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" ref="G67:G103" si="1">CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A67, ", '", B67, "', '", C67, "', ", IF(D67 = "", "NULL", CONCATENATE("'", D67, "'")), ", ", IF(E67 = "", "NULL", CONCATENATE("'", E67, "'")), ")")</f>
+        <f t="shared" ref="G67:G114" si="1">CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A67, ", '", B67, "', '", C67, "', ", IF(D67 = "", "NULL", CONCATENATE("'", D67, "'")), ", ", IF(E67 = "", "NULL", CONCATENATE("'", E67, "'")), ")")</f>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (66, 'rs104894504', 'short_text', 'rs104894504', 'dbSNP')</v>
       </c>
     </row>
@@ -2789,6 +2837,231 @@
       <c r="G103" t="str">
         <f t="shared" si="1"/>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (102, 'Genotype', 'short_text', 'Genotype', 'GVF')</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
+        <v>135</v>
+      </c>
+      <c r="C104" t="s">
+        <v>2</v>
+      </c>
+      <c r="G104" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (103, 'Variant Call Format result', 'binary', NULL, NULL)</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
+        <v>136</v>
+      </c>
+      <c r="C105" t="s">
+        <v>61</v>
+      </c>
+      <c r="D105" t="s">
+        <v>139</v>
+      </c>
+      <c r="E105" t="s">
+        <v>140</v>
+      </c>
+      <c r="G105" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (104, 'File Format', 'short_text', 'fileFormat', 'VCF')</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" t="s">
+        <v>137</v>
+      </c>
+      <c r="C106" t="s">
+        <v>61</v>
+      </c>
+      <c r="D106" t="s">
+        <v>138</v>
+      </c>
+      <c r="E106" t="s">
+        <v>140</v>
+      </c>
+      <c r="G106" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (105, 'Reference', 'short_text', 'reference', 'VCF')</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
+        <v>141</v>
+      </c>
+      <c r="C107" t="s">
+        <v>61</v>
+      </c>
+      <c r="D107" t="s">
+        <v>142</v>
+      </c>
+      <c r="E107" t="s">
+        <v>140</v>
+      </c>
+      <c r="G107" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (106, 'Phasing', 'short_text', 'phasing', 'VCF')</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" t="s">
+        <v>143</v>
+      </c>
+      <c r="C108" t="s">
+        <v>2</v>
+      </c>
+      <c r="D108" t="s">
+        <v>146</v>
+      </c>
+      <c r="E108" t="s">
+        <v>140</v>
+      </c>
+      <c r="G108" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (107, 'Information', 'binary', 'INFO', 'VCF')</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109" t="s">
+        <v>144</v>
+      </c>
+      <c r="C109" t="s">
+        <v>2</v>
+      </c>
+      <c r="D109" t="s">
+        <v>147</v>
+      </c>
+      <c r="E109" t="s">
+        <v>140</v>
+      </c>
+      <c r="G109" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (108, 'Filter', 'binary', 'FILTER', 'VCF')</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110" t="s">
+        <v>145</v>
+      </c>
+      <c r="C110" t="s">
+        <v>2</v>
+      </c>
+      <c r="D110" t="s">
+        <v>148</v>
+      </c>
+      <c r="E110" t="s">
+        <v>140</v>
+      </c>
+      <c r="G110" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (109, 'Format', 'binary', 'FORMAT', 'VCF')</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111" t="s">
+        <v>24</v>
+      </c>
+      <c r="C111" t="s">
+        <v>61</v>
+      </c>
+      <c r="D111" t="s">
+        <v>24</v>
+      </c>
+      <c r="E111" t="s">
+        <v>140</v>
+      </c>
+      <c r="G111" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (110, 'ID', 'short_text', 'ID', 'VCF')</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112" t="s">
+        <v>149</v>
+      </c>
+      <c r="C112" t="s">
+        <v>61</v>
+      </c>
+      <c r="D112" t="s">
+        <v>149</v>
+      </c>
+      <c r="E112" t="s">
+        <v>140</v>
+      </c>
+      <c r="G112" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (111, 'Number', 'short_text', 'Number', 'VCF')</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113" t="s">
+        <v>125</v>
+      </c>
+      <c r="C113" t="s">
+        <v>61</v>
+      </c>
+      <c r="D113" t="s">
+        <v>125</v>
+      </c>
+      <c r="E113" t="s">
+        <v>140</v>
+      </c>
+      <c r="G113" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (112, 'Type', 'short_text', 'Type', 'VCF')</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114" t="s">
+        <v>150</v>
+      </c>
+      <c r="C114" t="s">
+        <v>61</v>
+      </c>
+      <c r="D114" t="s">
+        <v>150</v>
+      </c>
+      <c r="E114" t="s">
+        <v>140</v>
+      </c>
+      <c r="G114" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (113, 'Description', 'short_text', 'Description', 'VCF')</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
VCF loader for EAV schema
</commit_message>
<xml_diff>
--- a/MHGR/Data/EAVAttributes/EAVAttributes.xlsx
+++ b/MHGR/Data/EAVAttributes/EAVAttributes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="176">
   <si>
     <t>Name</t>
   </si>
@@ -474,6 +474,81 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Variant Call Format variant</t>
+  </si>
+  <si>
+    <t>Reference base</t>
+  </si>
+  <si>
+    <t>Number of Samples With Data</t>
+  </si>
+  <si>
+    <t>Total Depth</t>
+  </si>
+  <si>
+    <t>Allele Frequency</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>Ancestral Allele</t>
+  </si>
+  <si>
+    <t>dbSNP membership, build 129</t>
+  </si>
+  <si>
+    <t>HapMap2 membership</t>
+  </si>
+  <si>
+    <t>Genotype Quality</t>
+  </si>
+  <si>
+    <t>Read Depth</t>
+  </si>
+  <si>
+    <t>INFO:NS</t>
+  </si>
+  <si>
+    <t>INFO:DP</t>
+  </si>
+  <si>
+    <t>INFO:AF</t>
+  </si>
+  <si>
+    <t>INFO:AA</t>
+  </si>
+  <si>
+    <t>INFO:DB</t>
+  </si>
+  <si>
+    <t>INFO:H2</t>
+  </si>
+  <si>
+    <t>FORMAT:GQ</t>
+  </si>
+  <si>
+    <t>FORMAT:GT</t>
+  </si>
+  <si>
+    <t>FORMAT:DP</t>
+  </si>
+  <si>
+    <t>FILTER:q10</t>
+  </si>
+  <si>
+    <t>FILTER:s50</t>
+  </si>
+  <si>
+    <t>q10 Filter</t>
+  </si>
+  <si>
+    <t>s50 Filter</t>
+  </si>
+  <si>
+    <t>Quality</t>
   </si>
 </sst>
 </file>
@@ -816,10 +891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G114"/>
+  <dimension ref="A1:G128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G112" sqref="G112"/>
+    <sheetView tabSelected="1" topLeftCell="C110" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F128" sqref="F128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2103,7 +2178,7 @@
         <v>66</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" ref="G67:G114" si="1">CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A67, ", '", B67, "', '", C67, "', ", IF(D67 = "", "NULL", CONCATENATE("'", D67, "'")), ", ", IF(E67 = "", "NULL", CONCATENATE("'", E67, "'")), ")")</f>
+        <f t="shared" ref="G67:G128" si="1">CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A67, ", '", B67, "', '", C67, "', ", IF(D67 = "", "NULL", CONCATENATE("'", D67, "'")), ", ", IF(E67 = "", "NULL", CONCATENATE("'", E67, "'")), ")")</f>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (66, 'rs104894504', 'short_text', 'rs104894504', 'dbSNP')</v>
       </c>
     </row>
@@ -3062,6 +3137,288 @@
       <c r="G114" t="str">
         <f t="shared" si="1"/>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (113, 'Description', 'short_text', 'Description', 'VCF')</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115" t="s">
+        <v>151</v>
+      </c>
+      <c r="C115" t="s">
+        <v>2</v>
+      </c>
+      <c r="G115" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (114, 'Variant Call Format variant', 'binary', NULL, NULL)</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
+        <v>152</v>
+      </c>
+      <c r="C116" t="s">
+        <v>61</v>
+      </c>
+      <c r="G116" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (115, 'Reference base', 'short_text', NULL, NULL)</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117" t="s">
+        <v>153</v>
+      </c>
+      <c r="C117" t="s">
+        <v>102</v>
+      </c>
+      <c r="D117" t="s">
+        <v>162</v>
+      </c>
+      <c r="E117" t="s">
+        <v>140</v>
+      </c>
+      <c r="G117" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (116, 'Number of Samples With Data', 'int', 'INFO:NS', 'VCF')</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118" t="s">
+        <v>154</v>
+      </c>
+      <c r="C118" t="s">
+        <v>102</v>
+      </c>
+      <c r="D118" t="s">
+        <v>163</v>
+      </c>
+      <c r="E118" t="s">
+        <v>140</v>
+      </c>
+      <c r="G118" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (117, 'Total Depth', 'int', 'INFO:DP', 'VCF')</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119" t="s">
+        <v>155</v>
+      </c>
+      <c r="C119" t="s">
+        <v>156</v>
+      </c>
+      <c r="D119" t="s">
+        <v>164</v>
+      </c>
+      <c r="E119" t="s">
+        <v>140</v>
+      </c>
+      <c r="G119" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (118, 'Allele Frequency', 'float', 'INFO:AF', 'VCF')</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120" t="s">
+        <v>157</v>
+      </c>
+      <c r="C120" t="s">
+        <v>61</v>
+      </c>
+      <c r="D120" t="s">
+        <v>165</v>
+      </c>
+      <c r="E120" t="s">
+        <v>140</v>
+      </c>
+      <c r="G120" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (119, 'Ancestral Allele', 'short_text', 'INFO:AA', 'VCF')</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121" t="s">
+        <v>158</v>
+      </c>
+      <c r="C121" t="s">
+        <v>2</v>
+      </c>
+      <c r="D121" t="s">
+        <v>166</v>
+      </c>
+      <c r="E121" t="s">
+        <v>140</v>
+      </c>
+      <c r="G121" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (120, 'dbSNP membership, build 129', 'binary', 'INFO:DB', 'VCF')</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122" t="s">
+        <v>159</v>
+      </c>
+      <c r="C122" t="s">
+        <v>2</v>
+      </c>
+      <c r="D122" t="s">
+        <v>167</v>
+      </c>
+      <c r="E122" t="s">
+        <v>140</v>
+      </c>
+      <c r="G122" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (121, 'HapMap2 membership', 'binary', 'INFO:H2', 'VCF')</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123" t="s">
+        <v>160</v>
+      </c>
+      <c r="C123" t="s">
+        <v>102</v>
+      </c>
+      <c r="D123" t="s">
+        <v>168</v>
+      </c>
+      <c r="E123" t="s">
+        <v>140</v>
+      </c>
+      <c r="G123" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (122, 'Genotype Quality', 'int', 'FORMAT:GQ', 'VCF')</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124" t="s">
+        <v>133</v>
+      </c>
+      <c r="C124" t="s">
+        <v>61</v>
+      </c>
+      <c r="D124" t="s">
+        <v>169</v>
+      </c>
+      <c r="E124" t="s">
+        <v>140</v>
+      </c>
+      <c r="G124" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (123, 'Genotype', 'short_text', 'FORMAT:GT', 'VCF')</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125" t="s">
+        <v>161</v>
+      </c>
+      <c r="C125" t="s">
+        <v>102</v>
+      </c>
+      <c r="D125" t="s">
+        <v>170</v>
+      </c>
+      <c r="E125" t="s">
+        <v>140</v>
+      </c>
+      <c r="G125" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (124, 'Read Depth', 'int', 'FORMAT:DP', 'VCF')</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126" t="s">
+        <v>173</v>
+      </c>
+      <c r="C126" t="s">
+        <v>2</v>
+      </c>
+      <c r="D126" t="s">
+        <v>171</v>
+      </c>
+      <c r="E126" t="s">
+        <v>140</v>
+      </c>
+      <c r="G126" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (125, 'q10 Filter', 'binary', 'FILTER:q10', 'VCF')</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127" t="s">
+        <v>174</v>
+      </c>
+      <c r="C127" t="s">
+        <v>2</v>
+      </c>
+      <c r="D127" t="s">
+        <v>172</v>
+      </c>
+      <c r="E127" t="s">
+        <v>140</v>
+      </c>
+      <c r="G127" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (126, 's50 Filter', 'binary', 'FILTER:s50', 'VCF')</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128" t="s">
+        <v>175</v>
+      </c>
+      <c r="C128" t="s">
+        <v>156</v>
+      </c>
+      <c r="D128" t="s">
+        <v>175</v>
+      </c>
+      <c r="E128" t="s">
+        <v>140</v>
+      </c>
+      <c r="G128" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (127, 'Quality', 'float', 'Quality', 'VCF')</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use more specific allele attribute types
</commit_message>
<xml_diff>
--- a/MHGR/Data/EAVAttributes/EAVAttributes.xlsx
+++ b/MHGR/Data/EAVAttributes/EAVAttributes.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\MHGR\MHGR\Data\EAVAttributes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\Documents\Thesis\MHGR\MHGR\Data\EAVAttributes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="5840" windowWidth="21360" windowHeight="5900"/>
+    <workbookView xWindow="-15" yWindow="5835" windowWidth="21360" windowHeight="5895" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="178">
   <si>
     <t>Name</t>
   </si>
@@ -549,6 +549,12 @@
   </si>
   <si>
     <t>Quality</t>
+  </si>
+  <si>
+    <t>Star allele</t>
+  </si>
+  <si>
+    <t>SNP allele</t>
   </si>
 </sst>
 </file>
@@ -891,21 +897,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G128"/>
+  <dimension ref="A1:G130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C110" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F128" sqref="F128"/>
+    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="48.90625" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -922,7 +927,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -937,7 +942,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (1, 'Relationship', 'binary', NULL, NULL)</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -952,7 +957,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (2, 'Is a', 'binary', NULL, NULL)</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -967,7 +972,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (3, 'Influenced by gene', 'binary', NULL, NULL)</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -982,7 +987,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (4, 'Influences phenotype', 'binary', NULL, NULL)</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -997,7 +1002,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (5, 'Variant of gene', 'binary', NULL, NULL)</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1012,7 +1017,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (6, 'Gene containing variant', 'binary', NULL, NULL)</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1027,7 +1032,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (7, 'Phenotype', 'binary', NULL, NULL)</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1042,7 +1047,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (8, 'Clopidogrel metabolism', 'binary', NULL, NULL)</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1057,7 +1062,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (9, 'Warfarin metabolism', 'binary', NULL, NULL)</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1072,7 +1077,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (10, 'Familial Thrombophilia', 'binary', NULL, NULL)</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1087,7 +1092,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (11, 'Hypertrophic Cardiomyopathy', 'binary', NULL, NULL)</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1102,7 +1107,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (12, 'Ultrarapid metabolizer', 'binary', NULL, NULL)</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1117,7 +1122,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (13, 'Extensive metabolizer', 'binary', NULL, NULL)</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1132,7 +1137,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (14, 'Intermediate metabolizer', 'binary', NULL, NULL)</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1147,7 +1152,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (15, 'Poor metabolizer', 'binary', NULL, NULL)</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1162,7 +1167,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (16, 'Normal', 'binary', NULL, NULL)</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1177,7 +1182,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (17, 'Decreased', 'binary', NULL, NULL)</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1198,7 +1203,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (18, 'Homozygous prothrombin G20210A mutation', 'binary', '289.81', 'ICD9-CM')</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1219,7 +1224,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (19, 'Heterozygous prothrombin G20210A mutation', 'binary', '289.81', 'ICD9-CM')</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1234,7 +1239,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (20, 'No genetic risk for prothrombin-related thrombophilia', 'binary', NULL, NULL)</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1255,7 +1260,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (21, 'Homozygous Factor V Leiden mutation', 'binary', '289.81', 'ICD9-CM')</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1276,7 +1281,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (22, 'Heterozygous Factor V Leiden mutation', 'binary', '289.81', 'ICD9-CM')</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1291,7 +1296,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (23, 'No genetic risk for thrombophilia, due to factor V Leiden', 'binary', NULL, NULL)</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1312,7 +1317,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (24, 'Double heterozygous for prothrombin G20210A mutation and Factor V Leiden mutation', 'binary', '289.81', 'ICD9-CM')</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1333,7 +1338,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (25, 'Cardiomyopathy, Familial Hypertrophic, 1', 'binary', '425.1', 'ICD9-CM')</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1354,7 +1359,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (26, 'Cardiomyopathy, Familial Hypertrophic, 2', 'binary', '425.1', 'ICD9-CM')</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1375,7 +1380,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (27, 'Cardiomyopathy, Familial Hypertrophic, 3', 'binary', '425.1', 'ICD9-CM')</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1396,7 +1401,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (28, 'Cardiomyopathy, Familial Hypertrophic, 4', 'binary', '425.1', 'ICD9-CM')</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1411,7 +1416,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (29, 'No genetic risk found', 'binary', NULL, NULL)</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1426,7 +1431,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (30, 'Gene', 'binary', NULL, NULL)</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1447,7 +1452,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (31, 'CYP2C19', 'binary', '2621', 'HGNC')</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1468,7 +1473,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (32, 'CYP2C9', 'binary', '2623', 'HGNC')</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1489,7 +1494,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (33, 'VKORC1', 'binary', '23663', 'HGNC')</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1510,7 +1515,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (34, 'F2', 'binary', '3535', 'HGNC')</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1531,7 +1536,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (35, 'F5', 'binary', '3542', 'HGNC')</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1552,7 +1557,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (36, 'MYH7', 'binary', '7577', 'HGNC')</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1573,7 +1578,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (37, 'MYBPC3', 'binary', '7551', 'HGNC')</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1594,7 +1599,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (38, 'TNNT2', 'binary', '11949', 'HGNC')</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1615,7 +1620,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (39, 'TPM1', 'binary', '12010', 'HGNC')</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1636,7 +1641,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (40, 'rs12248560', 'short_text', 'rs12248560', 'dbSNP')</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1657,7 +1662,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (41, 'rs28399504', 'short_text', 'rs28399504', 'dbSNP')</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1678,7 +1683,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (42, 'rs41291556', 'short_text', 'rs41291556', 'dbSNP')</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1699,7 +1704,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (43, 'rs72558184', 'short_text', 'rs72558184', 'dbSNP')</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1720,7 +1725,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (44, 'rs4986893', 'short_text', 'rs4986893', 'dbSNP')</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1741,7 +1746,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (45, 'rs4244285', 'short_text', 'rs4244285', 'dbSNP')</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1762,7 +1767,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (46, 'rs72558186', 'short_text', 'rs72558186', 'dbSNP')</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1783,7 +1788,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (47, 'rs56337013', 'short_text', 'rs56337013', 'dbSNP')</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1804,7 +1809,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (48, 'rs17884712', 'short_text', 'rs17884712', 'dbSNP')</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1825,7 +1830,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (49, 'rs6413438', 'short_text', 'rs6413438', 'dbSNP')</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1846,7 +1851,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (50, 'rs1057910', 'short_text', 'rs1057910', 'dbSNP')</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1867,7 +1872,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (51, 'rs1799853', 'short_text', 'rs1799853', 'dbSNP')</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1888,7 +1893,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (52, 'rs9923231', 'short_text', 'rs9923231', 'dbSNP')</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1909,7 +1914,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (53, 'rs9934438', 'short_text', 'rs9934438', 'dbSNP')</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1930,7 +1935,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (54, 'rs8050894', 'short_text', 'rs8050894', 'dbSNP')</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1951,7 +1956,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (55, 'rs6025', 'short_text', 'rs6025', 'dbSNP')</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1972,7 +1977,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (56, 'rs1799963', 'short_text', 'rs1799963', 'dbSNP')</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1993,7 +1998,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (57, 'rs121913626', 'short_text', 'rs121913626', 'dbSNP')</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2014,7 +2019,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (58, 'rs3218713', 'short_text', 'rs3218713', 'dbSNP')</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2035,7 +2040,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (59, 'rs3218714', 'short_text', 'rs3218714', 'dbSNP')</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2056,7 +2061,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (60, 'rs121964855', 'short_text', 'rs121964855', 'dbSNP')</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2077,7 +2082,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (61, 'rs121964856', 'short_text', 'rs121964856', 'dbSNP')</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2098,7 +2103,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (62, 'rs121964857', 'short_text', 'rs121964857', 'dbSNP')</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2119,7 +2124,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (63, 'rs28934269', 'short_text', 'rs28934269', 'dbSNP')</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2140,7 +2145,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (64, 'rs28934270', 'short_text', 'rs28934270', 'dbSNP')</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2161,7 +2166,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (65, 'rs727504290', 'short_text', 'rs727504290', 'dbSNP')</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2178,11 +2183,11 @@
         <v>66</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" ref="G67:G128" si="1">CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A67, ", '", B67, "', '", C67, "', ", IF(D67 = "", "NULL", CONCATENATE("'", D67, "'")), ", ", IF(E67 = "", "NULL", CONCATENATE("'", E67, "'")), ")")</f>
+        <f t="shared" ref="G67:G130" si="1">CONCATENATE("INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (", A67, ", '", B67, "', '", C67, "', ", IF(D67 = "", "NULL", CONCATENATE("'", D67, "'")), ", ", IF(E67 = "", "NULL", CONCATENATE("'", E67, "'")), ")")</f>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (66, 'rs104894504', 'short_text', 'rs104894504', 'dbSNP')</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2203,7 +2208,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (67, 'rs375882485', 'short_text', 'rs375882485', 'dbSNP')</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2224,7 +2229,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (68, 'rs397516083', 'short_text', 'rs397516083', 'dbSNP')</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2245,7 +2250,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (69, 'rs397515937', 'short_text', 'rs397515937', 'dbSNP')</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2266,7 +2271,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (70, 'rs397516074', 'short_text', 'rs397516074', 'dbSNP')</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2287,7 +2292,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (71, 'rs397515963', 'short_text', 'rs397515963', 'dbSNP')</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2302,7 +2307,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (72, 'Resulted on', 'date_time', NULL, NULL)</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2317,7 +2322,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (73, 'Allele', 'short_text', NULL, NULL)</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2332,7 +2337,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (74, 'Genomic Variant Format result', 'binary', NULL, NULL)</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2353,7 +2358,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (75, 'GVF Version', 'short_text', 'gvf-version', 'GVF')</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2374,7 +2379,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (76, 'GFF Version', 'short_text', 'gff-version', 'GVF')</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2395,7 +2400,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (77, 'File Version', 'short_text', 'file-version', 'GVF')</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2416,7 +2421,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (78, 'Source method', 'binary', 'source-method', 'GVF')</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2437,7 +2442,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (79, 'Source', 'short_text', 'Source', 'GVF')</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2458,7 +2463,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (80, 'Type', 'short_text', 'Type', 'GVF')</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2479,7 +2484,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (81, 'Dbxref', 'short_text', 'Dbxref', 'GVF')</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2500,7 +2505,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (82, 'Comment', 'text', 'Comment', 'GVF')</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2521,7 +2526,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (83, 'Technology platform', 'binary', 'technology-platform', 'GVF')</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2542,7 +2547,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (84, 'Platform class', 'short_text', 'Platform_class', 'GVF')</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2563,7 +2568,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (85, 'Platform name', 'short_text', 'Platform_name', 'GVF')</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2584,7 +2589,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (86, 'Read type', 'short_text', 'Read_type', 'GVF')</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2605,7 +2610,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (87, 'Read length', 'int', 'Read_length', 'GVF')</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2626,7 +2631,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (88, 'Read pair span', 'short_text', 'Read_pair_span', 'GVF')</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2647,7 +2652,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (89, 'Average coverage', 'int', 'Average_coverage', 'GVF')</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2668,7 +2673,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (90, 'Feature ontology', 'short_text', 'feature-ontology', 'GVF')</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2689,7 +2694,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (91, 'Genome build', 'short_text', 'genome-build', 'GVF')</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2710,7 +2715,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (92, 'Sequence region', 'binary', 'sequence-region', 'GVF')</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2731,7 +2736,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (93, 'Chromosome', 'short_text', 'Chromosome', 'GVF')</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2752,7 +2757,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (94, 'Start position', 'int', 'Start position', 'GVF')</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2773,7 +2778,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (95, 'End position', 'int', 'End position', 'GVF')</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2788,7 +2793,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (96, 'Genomic Variant Format feature', 'binary', NULL, NULL)</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2809,7 +2814,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (97, 'Score', 'short_text', 'Score', 'GVF')</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2830,7 +2835,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (98, 'Strand', 'short_text', 'Strand', 'GVF')</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -2851,7 +2856,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (99, 'Phase', 'short_text', 'Phase', 'GVF')</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -2872,7 +2877,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (100, 'Reference sequence', 'short_text', 'Reference_seq', 'GVF')</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -2893,7 +2898,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (101, 'Variant reads', 'short_text', 'Variant_reads', 'GVF')</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -2914,7 +2919,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (102, 'Genotype', 'short_text', 'Genotype', 'GVF')</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -2929,7 +2934,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (103, 'Variant Call Format result', 'binary', NULL, NULL)</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -2950,7 +2955,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (104, 'File Format', 'short_text', 'fileFormat', 'VCF')</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -2971,7 +2976,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (105, 'Reference', 'short_text', 'reference', 'VCF')</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -2992,7 +2997,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (106, 'Phasing', 'short_text', 'phasing', 'VCF')</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -3013,7 +3018,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (107, 'Information', 'binary', 'INFO', 'VCF')</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -3034,7 +3039,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (108, 'Filter', 'binary', 'FILTER', 'VCF')</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -3055,7 +3060,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (109, 'Format', 'binary', 'FORMAT', 'VCF')</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -3076,7 +3081,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (110, 'ID', 'short_text', 'ID', 'VCF')</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -3097,7 +3102,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (111, 'Number', 'short_text', 'Number', 'VCF')</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -3118,7 +3123,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (112, 'Type', 'short_text', 'Type', 'VCF')</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -3139,7 +3144,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (113, 'Description', 'short_text', 'Description', 'VCF')</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -3154,7 +3159,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (114, 'Variant Call Format variant', 'binary', NULL, NULL)</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -3169,7 +3174,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (115, 'Reference base', 'short_text', NULL, NULL)</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -3190,7 +3195,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (116, 'Number of Samples With Data', 'int', 'INFO:NS', 'VCF')</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -3211,7 +3216,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (117, 'Total Depth', 'int', 'INFO:DP', 'VCF')</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -3232,7 +3237,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (118, 'Allele Frequency', 'float', 'INFO:AF', 'VCF')</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -3253,7 +3258,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (119, 'Ancestral Allele', 'short_text', 'INFO:AA', 'VCF')</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -3274,7 +3279,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (120, 'dbSNP membership, build 129', 'binary', 'INFO:DB', 'VCF')</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -3295,7 +3300,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (121, 'HapMap2 membership', 'binary', 'INFO:H2', 'VCF')</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -3316,7 +3321,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (122, 'Genotype Quality', 'int', 'FORMAT:GQ', 'VCF')</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -3337,7 +3342,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (123, 'Genotype', 'short_text', 'FORMAT:GT', 'VCF')</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -3358,7 +3363,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (124, 'Read Depth', 'int', 'FORMAT:DP', 'VCF')</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -3379,7 +3384,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (125, 'q10 Filter', 'binary', 'FILTER:q10', 'VCF')</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -3400,7 +3405,7 @@
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (126, 's50 Filter', 'binary', 'FILTER:s50', 'VCF')</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
@@ -3419,6 +3424,36 @@
       <c r="G128" t="str">
         <f t="shared" si="1"/>
         <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (127, 'Quality', 'float', 'Quality', 'VCF')</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129" t="s">
+        <v>177</v>
+      </c>
+      <c r="C129" t="s">
+        <v>61</v>
+      </c>
+      <c r="G129" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (128, 'SNP allele', 'short_text', NULL, NULL)</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130" t="s">
+        <v>176</v>
+      </c>
+      <c r="C130" t="s">
+        <v>61</v>
+      </c>
+      <c r="G130" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attributes (id, name, value_type, code, code_system) VALUES (129, 'Star allele', 'short_text', NULL, NULL)</v>
       </c>
     </row>
   </sheetData>
@@ -3429,19 +3464,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:E123"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A123" sqref="A123"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -3452,7 +3487,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -3467,7 +3502,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (2, 1, 2)</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -3482,7 +3517,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (3, 1, 2)</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -3497,7 +3532,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (4, 1, 2)</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -3512,7 +3547,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (5, 1, 2)</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -3527,7 +3562,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (6, 1, 2)</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -3542,7 +3577,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (7, 1, 2)</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>30</v>
       </c>
@@ -3557,7 +3592,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (30, 1, 2)</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3572,7 +3607,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (8, 7, 2)</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3587,7 +3622,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (9, 7, 2)</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3602,7 +3637,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (10, 7, 2)</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3617,7 +3652,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (11, 7, 2)</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3632,7 +3667,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (12, 8, 2)</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3647,7 +3682,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (13, 8, 2)</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3662,7 +3697,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (14, 8, 2)</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3677,7 +3712,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (15, 8, 2)</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3692,7 +3727,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (16, 9, 2)</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3707,7 +3742,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (17, 9, 2)</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3722,7 +3757,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (18, 10, 2)</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3737,7 +3772,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (19, 10, 2)</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3752,7 +3787,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (20, 10, 2)</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3767,7 +3802,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (21, 10, 2)</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3782,7 +3817,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (22, 10, 2)</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3797,7 +3832,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (23, 10, 2)</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3812,7 +3847,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (24, 10, 2)</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3827,7 +3862,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (25, 11, 2)</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3842,7 +3877,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (26, 11, 2)</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3857,7 +3892,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (27, 11, 2)</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3872,7 +3907,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (28, 11, 2)</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3887,7 +3922,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (29, 11, 2)</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>31</v>
       </c>
@@ -3902,7 +3937,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 30, 2)</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>32</v>
       </c>
@@ -3917,7 +3952,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (32, 30, 2)</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>33</v>
       </c>
@@ -3932,7 +3967,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (33, 30, 2)</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>34</v>
       </c>
@@ -3947,7 +3982,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (34, 30, 2)</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>35</v>
       </c>
@@ -3962,7 +3997,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (35, 30, 2)</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>36</v>
       </c>
@@ -3977,7 +4012,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (36, 30, 2)</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>37</v>
       </c>
@@ -3992,7 +4027,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (37, 30, 2)</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>38</v>
       </c>
@@ -4007,7 +4042,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (38, 30, 2)</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>39</v>
       </c>
@@ -4022,7 +4057,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (39, 30, 2)</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>8</v>
       </c>
@@ -4037,7 +4072,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (8, 31, 3)</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>9</v>
       </c>
@@ -4052,7 +4087,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (9, 32, 3)</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>9</v>
       </c>
@@ -4067,7 +4102,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (9, 33, 3)</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>10</v>
       </c>
@@ -4082,7 +4117,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (10, 34, 3)</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>10</v>
       </c>
@@ -4097,7 +4132,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (10, 35, 3)</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>11</v>
       </c>
@@ -4112,7 +4147,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (11, 36, 3)</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>11</v>
       </c>
@@ -4127,7 +4162,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (11, 37, 3)</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>11</v>
       </c>
@@ -4142,7 +4177,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (11, 38, 3)</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>11</v>
       </c>
@@ -4157,7 +4192,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (11, 39, 3)</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>31</v>
       </c>
@@ -4172,7 +4207,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 8, 4)</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>32</v>
       </c>
@@ -4187,7 +4222,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (32, 9, 4)</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>33</v>
       </c>
@@ -4202,7 +4237,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (33, 9, 4)</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>34</v>
       </c>
@@ -4217,7 +4252,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (34, 10, 4)</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>35</v>
       </c>
@@ -4232,7 +4267,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (35, 10, 4)</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>36</v>
       </c>
@@ -4247,7 +4282,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (36, 11, 4)</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>37</v>
       </c>
@@ -4262,7 +4297,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (37, 11, 4)</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>38</v>
       </c>
@@ -4277,7 +4312,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (38, 11, 4)</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>39</v>
       </c>
@@ -4292,7 +4327,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (39, 11, 4)</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>40</v>
       </c>
@@ -4303,11 +4338,11 @@
         <v>5</v>
       </c>
       <c r="E58" t="str">
-        <f t="shared" ref="E58:E121" si="1">CONCATENATE("INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (", A58, ", ", B58, ", ", C58, ")")</f>
+        <f t="shared" ref="E58:E123" si="1">CONCATENATE("INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (", A58, ", ", B58, ", ", C58, ")")</f>
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (40, 31, 5)</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>41</v>
       </c>
@@ -4322,7 +4357,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (41, 31, 5)</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>42</v>
       </c>
@@ -4337,7 +4372,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (42, 31, 5)</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>43</v>
       </c>
@@ -4352,7 +4387,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (43, 31, 5)</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>44</v>
       </c>
@@ -4367,7 +4402,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (44, 31, 5)</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>45</v>
       </c>
@@ -4382,7 +4417,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (45, 31, 5)</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>46</v>
       </c>
@@ -4397,7 +4432,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (46, 31, 5)</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>47</v>
       </c>
@@ -4412,7 +4447,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (47, 31, 5)</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>48</v>
       </c>
@@ -4427,7 +4462,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (48, 31, 5)</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>49</v>
       </c>
@@ -4442,7 +4477,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (49, 31, 5)</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>50</v>
       </c>
@@ -4457,7 +4492,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (50, 32, 5)</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>51</v>
       </c>
@@ -4472,7 +4507,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (51, 32, 5)</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>52</v>
       </c>
@@ -4487,7 +4522,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (52, 33, 5)</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>53</v>
       </c>
@@ -4502,7 +4537,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (53, 33, 5)</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>54</v>
       </c>
@@ -4517,7 +4552,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (54, 33, 5)</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>55</v>
       </c>
@@ -4532,7 +4567,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (55, 35, 5)</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>56</v>
       </c>
@@ -4547,7 +4582,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (56, 34, 5)</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>57</v>
       </c>
@@ -4562,7 +4597,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (57, 36, 5)</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>58</v>
       </c>
@@ -4577,7 +4612,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (58, 36, 5)</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>59</v>
       </c>
@@ -4592,7 +4627,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (59, 36, 5)</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>60</v>
       </c>
@@ -4608,7 +4643,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (60, 38, 5)</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>61</v>
       </c>
@@ -4624,7 +4659,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (61, 38, 5)</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>62</v>
       </c>
@@ -4640,7 +4675,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (62, 38, 5)</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>63</v>
       </c>
@@ -4656,7 +4691,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (63, 39, 5)</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>64</v>
       </c>
@@ -4672,7 +4707,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (64, 39, 5)</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>65</v>
       </c>
@@ -4688,7 +4723,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (65, 39, 5)</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>66</v>
       </c>
@@ -4704,7 +4739,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (66, 39, 5)</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>67</v>
       </c>
@@ -4719,7 +4754,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (67, 37, 5)</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>68</v>
       </c>
@@ -4734,7 +4769,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (68, 37, 5)</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>69</v>
       </c>
@@ -4749,7 +4784,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (69, 37, 5)</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>70</v>
       </c>
@@ -4764,7 +4799,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (70, 37, 5)</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>71</v>
       </c>
@@ -4779,7 +4814,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (71, 37, 5)</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>31</v>
       </c>
@@ -4794,7 +4829,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 40, 6)</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>31</v>
       </c>
@@ -4809,7 +4844,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 41, 6)</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>31</v>
       </c>
@@ -4824,7 +4859,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 42, 6)</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>31</v>
       </c>
@@ -4839,7 +4874,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 43, 6)</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>31</v>
       </c>
@@ -4854,7 +4889,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 44, 6)</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>31</v>
       </c>
@@ -4869,7 +4904,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 45, 6)</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>31</v>
       </c>
@@ -4884,7 +4919,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 46, 6)</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>31</v>
       </c>
@@ -4899,7 +4934,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 47, 6)</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>31</v>
       </c>
@@ -4914,7 +4949,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 48, 6)</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>31</v>
       </c>
@@ -4929,7 +4964,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (31, 49, 6)</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>32</v>
       </c>
@@ -4944,7 +4979,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (32, 50, 6)</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>32</v>
       </c>
@@ -4959,7 +4994,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (32, 51, 6)</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>33</v>
       </c>
@@ -4974,7 +5009,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (33, 52, 6)</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>33</v>
       </c>
@@ -4989,7 +5024,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (33, 53, 6)</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>33</v>
       </c>
@@ -5004,7 +5039,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (33, 54, 6)</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>35</v>
       </c>
@@ -5019,7 +5054,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (35, 55, 6)</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>34</v>
       </c>
@@ -5034,7 +5069,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (34, 56, 6)</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>36</v>
       </c>
@@ -5049,7 +5084,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (36, 57, 6)</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>36</v>
       </c>
@@ -5064,7 +5099,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (36, 58, 6)</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>36</v>
       </c>
@@ -5079,7 +5114,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (36, 59, 6)</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>38</v>
       </c>
@@ -5094,7 +5129,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (38, 60, 6)</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>38</v>
       </c>
@@ -5109,7 +5144,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (38, 61, 6)</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>38</v>
       </c>
@@ -5124,7 +5159,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (38, 62, 6)</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>39</v>
       </c>
@@ -5139,7 +5174,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (39, 63, 6)</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>39</v>
       </c>
@@ -5154,7 +5189,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (39, 64, 6)</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>39</v>
       </c>
@@ -5169,7 +5204,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (39, 65, 6)</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>39</v>
       </c>
@@ -5184,7 +5219,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (39, 66, 6)</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>37</v>
       </c>
@@ -5199,7 +5234,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (37, 67, 6)</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>37</v>
       </c>
@@ -5214,7 +5249,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (37, 68, 6)</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>37</v>
       </c>
@@ -5229,7 +5264,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (37, 69, 6)</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>37</v>
       </c>
@@ -5244,7 +5279,7 @@
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (37, 70, 6)</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>37</v>
       </c>
@@ -5257,6 +5292,36 @@
       <c r="E121" t="str">
         <f t="shared" si="1"/>
         <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (37, 71, 6)</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>128</v>
+      </c>
+      <c r="B122">
+        <v>73</v>
+      </c>
+      <c r="C122">
+        <v>2</v>
+      </c>
+      <c r="E122" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (128, 73, 2)</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>129</v>
+      </c>
+      <c r="B123">
+        <v>73</v>
+      </c>
+      <c r="C123">
+        <v>2</v>
+      </c>
+      <c r="E123" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO dbo.attribute_relationships (attribute1_id, attribute2_id, relationship_id) VALUES (129, 73, 2)</v>
       </c>
     </row>
   </sheetData>
@@ -5270,7 +5335,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>